<commit_message>
Add sapmle data from table 4 to excel file.
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="107">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -331,6 +331,30 @@
   </si>
   <si>
     <t xml:space="preserve">Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:t-stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:pT1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:pT1b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:pT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:pT3a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:pT3b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:pT3c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:pT4</t>
   </si>
 </sst>
 </file>
@@ -346,6 +370,7 @@
       <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -531,7 +556,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -600,10 +625,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="22" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -626,10 +647,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -750,7 +767,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.62890625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.01"/>
@@ -831,7 +848,7 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -3931,10 +3948,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3949,7 +3966,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="14.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="40.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="40.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4003,7 +4020,7 @@
       <c r="C2" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E2" s="10" t="n">
@@ -4022,7 +4039,7 @@
       <c r="L2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="18"/>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
@@ -4032,7 +4049,7 @@
         <v>50</v>
       </c>
       <c r="C3" s="16"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E3" s="0" t="n">
@@ -4049,7 +4066,7 @@
       <c r="L3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="M3" s="18"/>
+      <c r="M3" s="17"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
@@ -4059,10 +4076,10 @@
         <v>28</v>
       </c>
       <c r="C4" s="16"/>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="19" t="n">
+      <c r="E4" s="18" t="n">
         <v>0</v>
       </c>
       <c r="F4" s="3"/>
@@ -4076,7 +4093,7 @@
       <c r="L4" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="M4" s="18"/>
+      <c r="M4" s="17"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
@@ -4086,10 +4103,10 @@
         <v>55</v>
       </c>
       <c r="C5" s="16"/>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="20" t="n">
+      <c r="E5" s="19" t="n">
         <v>0.25157</v>
       </c>
       <c r="F5" s="3"/>
@@ -4103,7 +4120,7 @@
       <c r="L5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="18"/>
+      <c r="M5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
@@ -4113,10 +4130,10 @@
         <v>58</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="20" t="n">
+      <c r="E6" s="19" t="n">
         <v>1.11962</v>
       </c>
       <c r="F6" s="3"/>
@@ -4130,13 +4147,13 @@
       <c r="L6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M6" s="18"/>
+      <c r="M6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="16"/>
-      <c r="D7" s="22"/>
+      <c r="D7" s="21"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -4145,7 +4162,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="18"/>
+      <c r="M7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
@@ -4154,10 +4171,10 @@
       <c r="B8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="20" t="s">
         <v>62</v>
       </c>
       <c r="E8" s="10" t="n">
@@ -4176,7 +4193,7 @@
       <c r="L8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="M8" s="18"/>
+      <c r="M8" s="17"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
@@ -4185,8 +4202,8 @@
       <c r="B9" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="24" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="20" t="s">
         <v>65</v>
       </c>
       <c r="E9" s="10" t="n">
@@ -4203,7 +4220,7 @@
       <c r="L9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="M9" s="18"/>
+      <c r="M9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
@@ -4212,8 +4229,8 @@
       <c r="B10" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24" t="s">
+      <c r="C10" s="22"/>
+      <c r="D10" s="20" t="s">
         <v>68</v>
       </c>
       <c r="E10" s="10" t="n">
@@ -4230,7 +4247,7 @@
       <c r="L10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M10" s="18"/>
+      <c r="M10" s="17"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
@@ -4239,8 +4256,8 @@
       <c r="B11" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="20" t="s">
         <v>71</v>
       </c>
       <c r="E11" s="10" t="n">
@@ -4257,13 +4274,13 @@
       <c r="L11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="M11" s="18"/>
+      <c r="M11" s="17"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -4272,7 +4289,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="18"/>
+      <c r="M12" s="17"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
@@ -4281,10 +4298,10 @@
       <c r="B13" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
         <v>75</v>
       </c>
       <c r="E13" s="10" t="n">
@@ -4303,7 +4320,7 @@
       <c r="L13" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="M13" s="18"/>
+      <c r="M13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
@@ -4312,20 +4329,20 @@
       <c r="B14" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27" t="s">
+      <c r="C14" s="24"/>
+      <c r="D14" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="19" t="n">
+      <c r="E14" s="18" t="n">
         <v>0.63358</v>
       </c>
       <c r="I14" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="L14" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="M14" s="18"/>
+      <c r="M14" s="17"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
@@ -4334,11 +4351,11 @@
       <c r="B15" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="27" t="s">
+      <c r="C15" s="26"/>
+      <c r="D15" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="19" t="n">
+      <c r="E15" s="18" t="n">
         <v>0.63358</v>
       </c>
       <c r="I15" s="3" t="n">
@@ -4347,7 +4364,7 @@
       <c r="L15" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M15" s="18"/>
+      <c r="M15" s="17"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
@@ -4356,11 +4373,11 @@
       <c r="B16" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="27" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="19" t="n">
+      <c r="E16" s="18" t="n">
         <v>0.63358</v>
       </c>
       <c r="I16" s="3" t="n">
@@ -4369,23 +4386,23 @@
       <c r="L16" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M16" s="18"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="26"/>
-      <c r="D17" s="22"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="21"/>
     </row>
     <row r="18" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="28" t="s">
         <v>86</v>
       </c>
       <c r="E18" s="10" t="n">
@@ -4395,7 +4412,7 @@
         <v>48</v>
       </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="31" t="s">
+      <c r="H18" s="29" t="s">
         <v>87</v>
       </c>
       <c r="I18" s="3" t="n">
@@ -4415,11 +4432,11 @@
       <c r="A19" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="30" t="s">
+      <c r="C19" s="24"/>
+      <c r="D19" s="28" t="s">
         <v>90</v>
       </c>
       <c r="E19" s="10" t="n">
@@ -4445,11 +4462,11 @@
       <c r="A20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="30" t="s">
+      <c r="C20" s="24"/>
+      <c r="D20" s="28" t="s">
         <v>92</v>
       </c>
       <c r="E20" s="10" t="n">
@@ -4475,11 +4492,11 @@
       <c r="A21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="32" t="s">
+      <c r="C21" s="24"/>
+      <c r="D21" s="30" t="s">
         <v>95</v>
       </c>
       <c r="E21" s="10" t="n">
@@ -4505,11 +4522,11 @@
       <c r="A22" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="32" t="s">
+      <c r="C22" s="24"/>
+      <c r="D22" s="30" t="s">
         <v>98</v>
       </c>
       <c r="E22" s="10" t="n">
@@ -4530,8 +4547,67 @@
       <c r="L22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Add data from table 4 to excel file.
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="119">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -339,22 +339,58 @@
     <t xml:space="preserve">:pT1a</t>
   </si>
   <si>
+    <t xml:space="preserve">[’p ‘TBD:]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pT1a</t>
+  </si>
+  <si>
     <t xml:space="preserve">:pT1b</t>
   </si>
   <si>
+    <t xml:space="preserve">1,24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pT1b</t>
+  </si>
+  <si>
     <t xml:space="preserve">:pT2</t>
   </si>
   <si>
+    <t xml:space="preserve">1,64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pT2</t>
+  </si>
+  <si>
     <t xml:space="preserve">:pT3a</t>
   </si>
   <si>
+    <t xml:space="preserve">1,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pT3a</t>
+  </si>
+  <si>
     <t xml:space="preserve">:pT3b</t>
   </si>
   <si>
+    <t xml:space="preserve">2,01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pT3b</t>
+  </si>
+  <si>
     <t xml:space="preserve">:pT3c</t>
   </si>
   <si>
+    <t xml:space="preserve">pT3c</t>
+  </si>
+  <si>
     <t xml:space="preserve">:pT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pT4</t>
   </si>
 </sst>
 </file>
@@ -3950,8 +3986,12 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="L30" activeCellId="0" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4560,53 +4600,122 @@
       <c r="D24" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="E25" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L25" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E26" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="E27" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="E28" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="E29" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>4</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>-50</v>
+      </c>
+      <c r="L30" s="0" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more data to excel file from table 4.
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="152">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -339,48 +339,100 @@
     <t xml:space="preserve">:pT1a</t>
   </si>
   <si>
-    <t xml:space="preserve">[’p ‘TBD:]</t>
+    <t xml:space="preserve">Primary tumor status</t>
   </si>
   <si>
     <t xml:space="preserve">pT1a</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[:p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">TBD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">]</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">:pT1b</t>
   </si>
   <si>
-    <t xml:space="preserve">1,24</t>
-  </si>
-  <si>
     <t xml:space="preserve">pT1b</t>
   </si>
   <si>
+    <t xml:space="preserve">1,243</t>
+  </si>
+  <si>
     <t xml:space="preserve">:pT2</t>
   </si>
   <si>
-    <t xml:space="preserve">1,64</t>
-  </si>
-  <si>
     <t xml:space="preserve">pT2</t>
   </si>
   <si>
+    <t xml:space="preserve">1,648</t>
+  </si>
+  <si>
     <t xml:space="preserve">:pT3a</t>
   </si>
   <si>
-    <t xml:space="preserve">1,8</t>
-  </si>
-  <si>
     <t xml:space="preserve">pT3a</t>
   </si>
   <si>
+    <t xml:space="preserve">1,896</t>
+  </si>
+  <si>
     <t xml:space="preserve">:pT3b</t>
   </si>
   <si>
-    <t xml:space="preserve">2,01</t>
-  </si>
-  <si>
     <t xml:space="preserve">pT3b</t>
   </si>
   <si>
+    <t xml:space="preserve">2,014</t>
+  </si>
+  <si>
     <t xml:space="preserve">:pT3c</t>
   </si>
   <si>
@@ -391,6 +443,146 @@
   </si>
   <si>
     <t xml:space="preserve">pT4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:n-stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:pNx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regional lymph node status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pNx</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[:p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">TBD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">:pN0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pN0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:pN1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pN1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:pN2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pN2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:tumor-size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:cm-&lt;10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tumor size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Less than 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cm-&lt;10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:cm-&gt;10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 or more</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,393</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cm→10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:nuclear-grade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuclear grade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,313</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:histologic-tumor-necrosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Histologic tumor necrosis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,678</t>
   </si>
 </sst>
 </file>
@@ -400,7 +592,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -466,6 +658,18 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -592,7 +796,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -717,6 +921,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3984,14 +4192,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="L30" activeCellId="0" sqref="L30"/>
+      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="D46" activeCellId="0" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4432,7 +4640,7 @@
       <c r="C17" s="24"/>
       <c r="D17" s="21"/>
     </row>
-    <row r="18" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="797.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
         <v>33</v>
       </c>
@@ -4590,15 +4798,18 @@
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>99</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="0" t="n">
-        <v>0</v>
+      <c r="C24" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>102</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>0</v>
@@ -4607,7 +4818,7 @@
         <v>48</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>50</v>
@@ -4617,14 +4828,17 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>99</v>
+      </c>
       <c r="B25" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>2</v>
+        <v>104</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>50</v>
@@ -4634,14 +4848,17 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>99</v>
+      </c>
       <c r="B26" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>3</v>
+        <v>107</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>108</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>50</v>
@@ -4651,14 +4868,17 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>99</v>
+      </c>
       <c r="B27" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>4</v>
+        <v>110</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>111</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>50</v>
@@ -4668,14 +4888,17 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>99</v>
+      </c>
       <c r="B28" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>4</v>
+        <v>113</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>114</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>50</v>
@@ -4685,37 +4908,343 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>99</v>
+      </c>
       <c r="B29" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>113</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>50</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>99</v>
+      </c>
       <c r="B30" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="D30" s="0" t="n">
+        <v>118</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L30" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="L32" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="L33" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="L34" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H40" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L40" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L42" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D43" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E30" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>-50</v>
-      </c>
-      <c r="L30" s="0" t="s">
-        <v>118</v>
+      <c r="E43" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L43" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="L45" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="L46" s="0" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add score column from table 4 to excel file.
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="151">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t xml:space="preserve">Things to consider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:score</t>
   </si>
   <si>
     <t xml:space="preserve">:18+</t>
@@ -457,53 +460,6 @@
     <t xml:space="preserve">pNx</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[:p </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">TBD</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">]</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">:pN0</t>
   </si>
   <si>
@@ -537,10 +493,7 @@
     <t xml:space="preserve">Less than 10</t>
   </si>
   <si>
-    <t xml:space="preserve">cm-&lt;10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:cm-&gt;10</t>
+    <t xml:space="preserve">:cm-&gt;=10</t>
   </si>
   <si>
     <t xml:space="preserve">10 or more</t>
@@ -549,7 +502,7 @@
     <t xml:space="preserve">0,393</t>
   </si>
   <si>
-    <t xml:space="preserve">Cm→10</t>
+    <t xml:space="preserve">Cm&gt;=10</t>
   </si>
   <si>
     <t xml:space="preserve">:nuclear-grade</t>
@@ -592,7 +545,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -658,18 +611,6 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -921,7 +862,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1008,7 +949,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="L37 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1093,7 +1034,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="L37 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1167,7 +1108,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H46" activeCellId="0" sqref="H46"/>
+      <selection pane="topLeft" activeCell="H46" activeCellId="1" sqref="L37 H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1219,7 +1160,7 @@
   <dimension ref="A1:C304"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F240" activeCellId="0" sqref="F240"/>
+      <selection pane="topLeft" activeCell="F240" activeCellId="1" sqref="L37 F240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4112,7 +4053,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="L37 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4192,14 +4133,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="D46" activeCellId="0" sqref="D46"/>
+      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="L37" activeCellId="0" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4257,25 +4198,28 @@
       <c r="M1" s="14" t="s">
         <v>44</v>
       </c>
+      <c r="N1" s="0" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" s="10" t="n">
         <v>-0.91329</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4285,7 +4229,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M2" s="17"/>
     </row>
@@ -4294,11 +4238,11 @@
         <v>27</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>-0.74681</v>
@@ -4312,7 +4256,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M3" s="17"/>
     </row>
@@ -4325,7 +4269,7 @@
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E4" s="18" t="n">
         <v>0</v>
@@ -4339,7 +4283,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="M4" s="17"/>
     </row>
@@ -4348,11 +4292,11 @@
         <v>27</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E5" s="19" t="n">
         <v>0.25157</v>
@@ -4366,7 +4310,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M5" s="17"/>
     </row>
@@ -4375,11 +4319,11 @@
         <v>27</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E6" s="19" t="n">
         <v>1.11962</v>
@@ -4393,7 +4337,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M6" s="17"/>
     </row>
@@ -4420,16 +4364,16 @@
         <v>31</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" s="10" t="n">
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -4439,7 +4383,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M8" s="17"/>
     </row>
@@ -4448,11 +4392,11 @@
         <v>30</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E9" s="10" t="n">
         <v>0.19494</v>
@@ -4466,7 +4410,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M9" s="17"/>
     </row>
@@ -4475,11 +4419,11 @@
         <v>30</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E10" s="10" t="n">
         <v>0.33312</v>
@@ -4493,7 +4437,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M10" s="17"/>
     </row>
@@ -4502,11 +4446,11 @@
         <v>30</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E11" s="10" t="n">
         <v>0.72515</v>
@@ -4520,7 +4464,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M11" s="17"/>
     </row>
@@ -4544,19 +4488,19 @@
         <v>32</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E13" s="10" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -4566,7 +4510,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M13" s="17"/>
     </row>
@@ -4575,11 +4519,11 @@
         <v>32</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E14" s="18" t="n">
         <v>0.63358</v>
@@ -4588,7 +4532,7 @@
         <v>20</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M14" s="17"/>
     </row>
@@ -4597,11 +4541,11 @@
         <v>32</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E15" s="18" t="n">
         <v>0.63358</v>
@@ -4610,7 +4554,7 @@
         <v>20</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M15" s="17"/>
     </row>
@@ -4619,11 +4563,11 @@
         <v>32</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C16" s="26"/>
       <c r="D16" s="25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E16" s="18" t="n">
         <v>0.63358</v>
@@ -4632,7 +4576,7 @@
         <v>20</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M16" s="17"/>
     </row>
@@ -4645,35 +4589,35 @@
         <v>33</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E18" s="10" t="n">
         <v>0.20284</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I18" s="3" t="n">
         <v>40</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4681,11 +4625,11 @@
         <v>33</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C19" s="24"/>
       <c r="D19" s="28" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E19" s="10" t="n">
         <v>0.07945</v>
@@ -4697,13 +4641,13 @@
         <v>40</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4715,7 +4659,7 @@
       </c>
       <c r="C20" s="24"/>
       <c r="D20" s="28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E20" s="10" t="n">
         <v>0</v>
@@ -4727,13 +4671,13 @@
         <v>40</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4741,11 +4685,11 @@
         <v>33</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C21" s="24"/>
       <c r="D21" s="30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E21" s="10" t="n">
         <v>-0.31232</v>
@@ -4757,13 +4701,13 @@
         <v>40</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4771,11 +4715,11 @@
         <v>33</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C22" s="24"/>
       <c r="D22" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E22" s="10" t="n">
         <v>-0.31232</v>
@@ -4787,10 +4731,10 @@
         <v>40</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L22" s="3"/>
     </row>
@@ -4800,185 +4744,209 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>50</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>50</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>50</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>50</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>50</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B29" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>115</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>50</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>50</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H32" s="31" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>60</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>125</v>
@@ -4990,7 +4958,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>60</v>
@@ -4998,10 +4966,13 @@
       <c r="L33" s="0" t="s">
         <v>126</v>
       </c>
+      <c r="N33" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>127</v>
@@ -5013,7 +4984,7 @@
         <v>129</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>60</v>
@@ -5021,10 +4992,13 @@
       <c r="L34" s="0" t="s">
         <v>128</v>
       </c>
+      <c r="N34" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>130</v>
@@ -5036,13 +5010,16 @@
         <v>129</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I35" s="0" t="n">
         <v>60</v>
       </c>
       <c r="L35" s="0" t="s">
         <v>131</v>
+      </c>
+      <c r="N35" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5062,16 +5039,16 @@
         <v>0</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H37" s="31" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="I37" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="L37" s="0" t="s">
-        <v>136</v>
+      <c r="N37" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5079,33 +5056,36 @@
         <v>132</v>
       </c>
       <c r="B38" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="E38" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="E38" s="0" t="s">
-        <v>139</v>
-      </c>
       <c r="F38" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>70</v>
       </c>
       <c r="L38" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="N38" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>142</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>1</v>
@@ -5114,10 +5094,10 @@
         <v>0</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H40" s="31" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="I40" s="0" t="n">
         <v>80</v>
@@ -5125,13 +5105,16 @@
       <c r="L40" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="N40" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>2</v>
@@ -5140,7 +5123,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I41" s="0" t="n">
         <v>80</v>
@@ -5148,10 +5131,13 @@
       <c r="L41" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="N41" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>34</v>
@@ -5160,10 +5146,10 @@
         <v>3</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>80</v>
@@ -5171,22 +5157,25 @@
       <c r="L42" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="N42" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>4</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I43" s="0" t="n">
         <v>80</v>
@@ -5194,59 +5183,69 @@
       <c r="L43" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="N43" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="C45" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="D45" s="0" t="s">
         <v>147</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>148</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H45" s="31" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>90</v>
       </c>
       <c r="L45" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="N45" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" s="0" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B46" s="0" t="s">
+      <c r="D46" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="E46" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="E46" s="0" t="s">
-        <v>151</v>
-      </c>
       <c r="F46" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>90</v>
       </c>
       <c r="L46" s="0" t="s">
-        <v>150</v>
-      </c>
-    </row>
+        <v>149</v>
+      </c>
+      <c r="N46" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Remove all extra widgets.
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="82">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -132,97 +132,19 @@
     <t xml:space="preserve">:3</t>
   </si>
   <si>
-    <t xml:space="preserve">:factor-name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:level-name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:beta-ldsurvival</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:sub-text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:info-box?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:boxed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:r-name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Things to consider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:18+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 - 29</t>
+    <t xml:space="preserve">:t-stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:pT1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary tumor status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pT1a</t>
   </si>
   <si>
     <t xml:space="preserve">:v-radio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rage_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:30+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 - 39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rage_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40 - 49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rage_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:50+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50 - 59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rage_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:60+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60 or over</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rage_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:t-stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:pT1a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary tumor status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pT1a</t>
   </si>
   <si>
     <r>
@@ -407,7 +329,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -467,15 +389,8 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Grande"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -500,35 +415,11 @@
         <bgColor rgb="FFF4B183"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2F0D9"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium">
-        <color rgb="FF00B0F0"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium">
-        <color rgb="FF00B0F0"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -570,7 +461,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -620,42 +511,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="22" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -709,9 +564,9 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00B0F0"/>
+      <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFE2F0D9"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFF4B084"/>
@@ -3937,12 +3792,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43"/>
@@ -3955,427 +3810,371 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="40.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="13" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="D1" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="E1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="13" t="s">
+      <c r="D2" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="E2" s="0" t="n">
+        <v>1.243</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="D3" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="E3" s="0" t="n">
+        <v>1.648</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="15" t="s">
+      <c r="D4" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="E4" s="0" t="n">
+        <v>1.896</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D5" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="10" t="n">
-        <v>-0.91329</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E5" s="0" t="n">
+        <v>2.014</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="D6" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="17"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="E6" s="0" t="n">
+        <v>2.014</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="3" t="s">
+      <c r="D7" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>-0.74681</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3" t="s">
+      <c r="E7" s="0" t="n">
+        <v>2.014</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M3" s="17"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="3" t="s">
+      <c r="B9" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="18" t="n">
+      <c r="C9" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="17"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="15" t="s">
+      <c r="F9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="L9" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="19" t="n">
-        <v>0.25157</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" s="17"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="19" t="n">
-        <v>1.11962</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M6" s="17"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="17"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="0" t="n">
+      <c r="N9" s="0" t="n">
         <v>0</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="N8" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>1.243</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="N9" s="0" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1.648</v>
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="I10" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="N10" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>1.896</v>
+        <v>0.924</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="N11" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="E12" s="0" t="n">
+        <v>0.924</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>0.393</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>2.014</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="N12" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>2.014</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="N13" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>2.014</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="N14" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="L16" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="N16" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>84</v>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>49</v>
+        <v>39</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="I17" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="N17" s="0" t="n">
         <v>0</v>
@@ -4383,283 +4182,148 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>86</v>
+        <v>74</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>0.924</v>
+        <v>0</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="I18" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>86</v>
+        <v>80</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="N18" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1.313</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <v>0.924</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I19" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="L19" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="N19" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="0" t="s">
+      <c r="E22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="0" t="n">
+      <c r="L22" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="N22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F21" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H21" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="N21" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>0.393</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="L22" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="N22" s="0" t="n">
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0.678</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="N23" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="L24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N24" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="L25" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="N25" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I26" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="L26" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N26" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>1.313</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I27" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="L27" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="N27" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H29" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="I29" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="L29" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="N29" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>0.678</v>
-      </c>
-      <c r="F30" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="L30" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="N30" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Fix start tool button problem & Minor changes in excel file.
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="93">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -130,6 +130,39 @@
   </si>
   <si>
     <t xml:space="preserve">:3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:factor-name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:level-name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:beta-ldsurvival</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:sub-text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:info-box?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:boxed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:r-name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Things to consider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:score</t>
   </si>
   <si>
     <t xml:space="preserve">:t-stage</t>
@@ -390,7 +423,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,6 +446,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF8CBAD"/>
         <bgColor rgb="FFF4B183"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2F0D9"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -461,7 +500,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -511,6 +550,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -566,7 +613,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFE2F0D9"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFF4B084"/>
@@ -3792,12 +3839,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43"/>
@@ -3810,125 +3857,146 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="40.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="E1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="F1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="0" t="n">
+      <c r="G1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="0" t="n">
+      <c r="F2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="N1" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>1.243</v>
+      <c r="H2" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>50</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>1.648</v>
+        <v>1.243</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>50</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>1.896</v>
+        <v>1.648</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>50</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>2.014</v>
+        <v>1.896</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>50</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>4</v>
@@ -3936,13 +4004,13 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>2.014</v>
@@ -3951,7 +4019,7 @@
         <v>50</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>4</v>
@@ -3959,13 +4027,13 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>2.014</v>
@@ -3974,65 +4042,62 @@
         <v>50</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="N7" s="0" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="N9" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>2.014</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>39</v>
+        <v>50</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>60</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>0</v>
@@ -4040,167 +4105,167 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>0.924</v>
+        <v>0</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>60</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="N11" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>0.924</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>60</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="0" t="s">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="0" t="n">
+      <c r="B13" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0.924</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="N14" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>0.393</v>
-      </c>
       <c r="F15" s="0" t="s">
-        <v>39</v>
+        <v>50</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>70</v>
       </c>
       <c r="L15" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0.393</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="N15" s="0" t="n">
+      <c r="L16" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="N16" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="0" t="n">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="L17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N17" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>2</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>39</v>
+        <v>50</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>80</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>0</v>
@@ -4208,116 +4273,141 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>0.64</v>
+        <v>0</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>80</v>
       </c>
       <c r="L19" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N19" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>1.313</v>
+        <v>0.64</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>80</v>
       </c>
       <c r="L20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="N20" s="0" t="n">
+      <c r="E21" s="0" t="n">
+        <v>1.313</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N21" s="0" t="n">
         <v>3</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="H22" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="L22" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="N22" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>80</v>
+        <v>88</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>0.678</v>
+        <v>0</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>39</v>
+        <v>50</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>90</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="N23" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>0.678</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="N24" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add place-holder to tool page.
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="94">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -75,7 +75,7 @@
     <t xml:space="preserve">assets/kidney/osm_logo.svg</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the adult transplant centre where the patient will be receiving their transplant.  This is not always the same as the dialysis follow-up centre.</t>
+    <t xml:space="preserve">Placeholder-1</t>
   </si>
   <si>
     <t xml:space="preserve">:label</t>
@@ -165,187 +165,19 @@
     <t xml:space="preserve">:score</t>
   </si>
   <si>
-    <t xml:space="preserve">:18+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 - 29</t>
+    <t xml:space="preserve">:t-stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:pT1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary tumor status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pT1a</t>
   </si>
   <si>
     <t xml:space="preserve">:v-radio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rage_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:30+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 - 39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rage_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40 - 49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rage_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:50+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50 - 59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rage_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:60+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60 or over</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rage_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waiting time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">up to 6 months</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:mw-&lt;=12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 months to a year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:mw-&lt;=24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 to 2 years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:mw-24+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 years or more</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary kidney disease</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diabetes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diabetes_0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:pckd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCKD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diabetes_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:glo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glomerulonephritis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLA mismatch level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">⓵ (000)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[:&lt;&gt;
-[:p "HLA stands for Human Leukocyte Antigen."]
-[:p "HLA are proteins on the surface of white blood cells and other tissues."]
-[:p "When people have the same HLAs they are said to be a match. There are many different types of HLAs so matching can be to differing degrees.  Patients can match ‘a lot’ or ‘a little’."]
-[:p "HLA mismatch means how likely a patient is to be matched based on these HLA proteins"]
-[:p [:b "Level 1"] " 000"]
-[:p [:b "Level 2"] " [0 DR and 0/1 B] or [1 DR and 0 B]"]
-[:p [:b "Level 3"] " [0 DR and 2 B] or [1 DR and 1 B]"]
-[:p [:b "Level 4"] " [1 DR and 2 B] or [2 DR]"]
-]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hla_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">⓶ (100, 010, 110, 200, 210, 001,101, 201)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hla_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">⓷ (020, 120, 220, 011, 111, 211)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hla_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">⓸ (021, 121, 221, 002, 102, 202, 012, 112, 212, 022, 122, 222)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hla_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:t-stage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">:pT1a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary tumor status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pT1a</t>
   </si>
   <si>
     <r>
@@ -376,7 +208,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">TBD</t>
+      <t xml:space="preserve">Placeholder-7</t>
     </r>
     <r>
       <rPr>
@@ -493,7 +325,63 @@
     <t xml:space="preserve">:nuclear-grade</t>
   </si>
   <si>
+    <t xml:space="preserve">:1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nuclear grade</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[:p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Placeholder-7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">]</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">:2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:4</t>
   </si>
   <si>
     <t xml:space="preserve">:histologic-tumor-necrosis</t>
@@ -521,7 +409,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -582,11 +470,16 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Lucida Grande"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -621,59 +514,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium">
-        <color rgb="FF00B0F0"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium">
-        <color rgb="FF00B0F0"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium">
-        <color rgb="FF4472C4"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium">
-        <color rgb="FF4472C4"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium">
-        <color rgb="FF4472C4"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF4472C4"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -713,7 +559,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -774,71 +620,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="22" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -888,7 +674,7 @@
       <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00B0F0"/>
+      <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFE2F0D9"/>
       <rgbColor rgb="FFFFFF99"/>
@@ -896,7 +682,7 @@
       <rgbColor rgb="FFF4B084"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF8CBAD"/>
-      <rgbColor rgb="FF4472C4"/>
+      <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
@@ -1010,7 +796,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1135,7 +921,7 @@
   </sheetPr>
   <dimension ref="A1:C304"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A196" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F240" activeCellId="0" sqref="F240"/>
     </sheetView>
   </sheetViews>
@@ -4112,11 +3898,11 @@
   <dimension ref="A1:N1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A48" activeCellId="0" sqref="A48"/>
+      <selection pane="bottomRight" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4178,1053 +3964,535 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="15" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="10" t="n">
-        <v>-0.91329</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="D2" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="E2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="17"/>
+      <c r="H2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1.243</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1.648</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>1.896</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2.014</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2.014</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>2.014</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>-0.74681</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" s="17"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="18" t="n">
+      <c r="I10" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="N10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="M4" s="17"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="19" t="n">
-        <v>0.25157</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="M5" s="17"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="20" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="E6" s="19" t="n">
-        <v>1.11962</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="M6" s="17"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="17"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="10" t="n">
+      <c r="L11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="M8" s="17"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E9" s="10" t="n">
-        <v>0.19494</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="M9" s="17"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="10" t="n">
-        <v>0.33312</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3" t="s">
+      <c r="B12" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="17"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="D12" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="20" t="s">
+      <c r="E12" s="0" t="n">
+        <v>0.924</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="10" t="n">
-        <v>0.72515</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3" t="s">
+      <c r="D13" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="M11" s="17"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="17"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="15" t="s">
+      <c r="E13" s="0" t="n">
+        <v>0.924</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="B15" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="C15" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="10" t="n">
+      <c r="D15" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="M13" s="17"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="12" t="s">
+      <c r="F15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L15" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25" t="s">
+      <c r="N15" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="18" t="n">
-        <v>0.63358</v>
-      </c>
-      <c r="I14" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="L14" s="3" t="s">
+      <c r="D16" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="M14" s="17"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="12" t="s">
+      <c r="E16" s="0" t="n">
+        <v>0.393</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L16" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="25" t="s">
+      <c r="N16" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="18" t="n">
-        <v>0.63358</v>
-      </c>
-      <c r="I15" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="L15" s="5" t="s">
+      <c r="B18" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="M15" s="17"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="E16" s="18" t="n">
-        <v>0.63358</v>
-      </c>
-      <c r="I16" s="3" t="n">
-        <v>20</v>
-      </c>
-      <c r="L16" s="5" t="s">
+      <c r="L18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="M16" s="17"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="24"/>
-      <c r="D17" s="21"/>
-    </row>
-    <row r="18" customFormat="false" ht="797.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="27" t="s">
+      <c r="L19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>1.313</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="10" t="n">
-        <v>0.20284</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="I18" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="27" t="s">
+      <c r="I23" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="28" t="s">
+      <c r="L23" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="10" t="n">
-        <v>0.07945</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="E20" s="10" t="n">
+      <c r="N23" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="E21" s="10" t="n">
-        <v>-0.31232</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="10" t="n">
-        <v>-0.31232</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>0</v>
+        <v>0.678</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="I24" s="0" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="N24" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <v>1.243</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L25" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="N25" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <v>1.648</v>
-      </c>
-      <c r="I26" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L26" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="N26" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="E27" s="0" t="n">
-        <v>1.896</v>
-      </c>
-      <c r="I27" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L27" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="N27" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="E28" s="0" t="n">
-        <v>2.014</v>
-      </c>
-      <c r="I28" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L28" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="N28" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="0" t="n">
-        <v>2.014</v>
-      </c>
-      <c r="I29" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L29" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="N29" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>2.014</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="L30" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="N30" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="E32" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H32" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="I32" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="L32" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="N32" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I33" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="L33" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="N33" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>0.924</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I34" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="L34" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="N34" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>0.924</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I35" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="L35" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="N35" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="E37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H37" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="I37" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="L37" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="N37" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>0.393</v>
-      </c>
-      <c r="F38" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I38" s="0" t="n">
-        <v>70</v>
-      </c>
-      <c r="L38" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="N38" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="D40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E40" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H40" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="I40" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="L40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="N40" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I41" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="L41" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="N41" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>0.64</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I42" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="L42" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="N42" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D43" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E43" s="0" t="n">
-        <v>1.313</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I43" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="L43" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="N43" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H45" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="I45" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="L45" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="N45" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E46" s="0" t="n">
-        <v>0.678</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I46" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="L46" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="N46" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add excel file with months calculation.
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="93">
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
@@ -331,53 +331,6 @@
     <t xml:space="preserve">Nuclear grade</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[:p </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Placeholder-7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">]</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">:2</t>
   </si>
   <si>
@@ -406,10 +359,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0\٫000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -468,18 +422,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -600,6 +542,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -621,10 +567,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -711,7 +653,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="1" sqref="D87:D122 A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.62109375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -796,7 +738,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="D87:D122 F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -870,7 +812,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H46" activeCellId="0" sqref="H46"/>
+      <selection pane="topLeft" activeCell="H46" activeCellId="1" sqref="D87:D122 H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -919,17 +861,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C304"/>
+  <dimension ref="A1:S304"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A196" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F240" activeCellId="0" sqref="F240"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D87" activeCellId="0" sqref="D87:D122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,16 +902,29 @@
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <f aca="false">-(1-C14)/12</f>
+        <v>-0.000665077091402085</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>0.999732405</v>
+        <f aca="false">B2+1</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">D2+$E$2</f>
+        <v>0.999334922908598</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">($C$38-$C$14)/24</f>
+        <v>-0.000440094596224872</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -970,32 +932,50 @@
         <v>13</v>
       </c>
       <c r="B4" s="0" t="n">
+        <f aca="false">B3+1</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">D3+$E$2</f>
+        <v>0.998669845817196</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">($C$62-$C$38)/24</f>
+        <v>-0.00021672248282346</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">B4+1</f>
+        <v>3</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">D4+$E$2</f>
+        <v>0.998004768725794</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">($C$86-$C$62)/24</f>
+        <v>-0.000179834484951125</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <f aca="false">B5+1</f>
         <v>4</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>0.999598591</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>0.999464728</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>0.999330667</v>
+      <c r="D6" s="0" t="n">
+        <f aca="false">D5+$E$2</f>
+        <v>0.997339691634392</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">($C$122-$C$86)/36</f>
+        <v>-0.000150386302030391</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1003,10 +983,18 @@
         <v>13</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>0.999062355</v>
+        <f aca="false">B6+1</f>
+        <v>5</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">D6+$E$2</f>
+        <v>0.99667461454299</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,10 +1002,16 @@
         <v>13</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>0.998928062</v>
+        <f aca="false">B7+1</f>
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">D7+$E$2</f>
+        <v>0.996009537451588</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <f aca="false">R7+S$7</f>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1025,10 +1019,16 @@
         <v>13</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>0.998793671</v>
+        <f aca="false">B8+1</f>
+        <v>7</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <f aca="false">D8+$E$2</f>
+        <v>0.995344460360185</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <f aca="false">R8+S$7</f>
+        <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1036,10 +1036,34 @@
         <v>13</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>0.998524875</v>
+        <f aca="false">B9+1</f>
+        <v>8</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <f aca="false">D9+$E$2</f>
+        <v>0.994679383268784</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0.992019074903175</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>0.981456804593778</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.976255465006015</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.971939437367188</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>0.966525530494094</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <f aca="false">R9+S$7</f>
+        <v>4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,10 +1071,24 @@
         <v>13</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>0.998390338</v>
+        <f aca="false">B10+1</f>
+        <v>9</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <f aca="false">D10+$E$2</f>
+        <v>0.994014306177381</v>
+      </c>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10" t="n">
+        <f aca="false">P10*2</f>
+        <v>2</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <f aca="false">R10+S$7</f>
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1058,10 +1096,20 @@
         <v>13</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>24</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>0.99825578</v>
+        <f aca="false">B11+1</f>
+        <v>10</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <f aca="false">D11+$E$2</f>
+        <v>0.993349229085979</v>
+      </c>
+      <c r="P12" s="10" t="n">
+        <f aca="false">P11*2</f>
+        <v>4</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <f aca="false">R11+S$7</f>
+        <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1069,10 +1117,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>0.998121201</v>
+        <f aca="false">B12+1</f>
+        <v>11</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">D12+$E$2</f>
+        <v>0.992684151994577</v>
+      </c>
+      <c r="P13" s="10" t="n">
+        <f aca="false">P12*2</f>
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1080,10 +1134,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>34</v>
+        <f aca="false">B13+1</f>
+        <v>12</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>0.997986601</v>
+        <v>0.992019074903175</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">D13+$E$2</f>
+        <v>0.992019074903175</v>
+      </c>
+      <c r="P14" s="10" t="n">
+        <f aca="false">P13*2</f>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,21 +1154,37 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>0.997851964</v>
-      </c>
+        <f aca="false">B14+1</f>
+        <v>13</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">D14+$E$3</f>
+        <v>0.99157898030695</v>
+      </c>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10" t="n">
+        <f aca="false">P14*2</f>
+        <v>32</v>
+      </c>
+      <c r="Q15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>0.997717307</v>
+        <f aca="false">B15+1</f>
+        <v>14</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <f aca="false">D15+$E$3</f>
+        <v>0.991138885710726</v>
+      </c>
+      <c r="P16" s="10" t="n">
+        <f aca="false">P15*2</f>
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,10 +1192,16 @@
         <v>13</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>0.997582567</v>
+        <f aca="false">B16+1</f>
+        <v>15</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <f aca="false">D16+$E$3</f>
+        <v>0.990698791114501</v>
+      </c>
+      <c r="P17" s="10" t="n">
+        <f aca="false">P16*2</f>
+        <v>128</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1124,10 +1209,16 @@
         <v>13</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>0.997447827</v>
+        <f aca="false">B17+1</f>
+        <v>16</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <f aca="false">D17+$E$3</f>
+        <v>0.990258696518276</v>
+      </c>
+      <c r="P18" s="10" t="n">
+        <f aca="false">P17*2</f>
+        <v>256</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1135,10 +1226,16 @@
         <v>13</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>0.997313053</v>
+        <f aca="false">B18+1</f>
+        <v>17</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <f aca="false">D18+$E$3</f>
+        <v>0.989818601922051</v>
+      </c>
+      <c r="P19" s="10" t="n">
+        <f aca="false">P18*2</f>
+        <v>512</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1146,10 +1243,16 @@
         <v>13</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>63</v>
-      </c>
-      <c r="C20" s="0" t="n">
-        <v>0.997178266</v>
+        <f aca="false">B19+1</f>
+        <v>18</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">D19+$E$3</f>
+        <v>0.989378507325826</v>
+      </c>
+      <c r="P20" s="10" t="n">
+        <f aca="false">P19*2</f>
+        <v>1024</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1157,10 +1260,16 @@
         <v>13</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>64</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>0.997043481</v>
+        <f aca="false">B20+1</f>
+        <v>19</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">D20+$E$3</f>
+        <v>0.988938412729601</v>
+      </c>
+      <c r="P21" s="10" t="n">
+        <f aca="false">P20*2</f>
+        <v>2048</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1168,10 +1277,12 @@
         <v>13</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>77</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>0.996908183</v>
+        <f aca="false">B21+1</f>
+        <v>20</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">D21+$E$3</f>
+        <v>0.988498318133376</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,10 +1290,12 @@
         <v>13</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>78</v>
-      </c>
-      <c r="C23" s="0" t="n">
-        <v>0.99663739</v>
+        <f aca="false">B22+1</f>
+        <v>21</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">D22+$E$3</f>
+        <v>0.988058223537152</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,10 +1303,12 @@
         <v>13</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>83</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>0.996501731</v>
+        <f aca="false">B23+1</f>
+        <v>22</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">D23+$E$3</f>
+        <v>0.987618128940927</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1201,10 +1316,12 @@
         <v>13</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>84</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>0.996365972</v>
+        <f aca="false">B24+1</f>
+        <v>23</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">D24+$E$3</f>
+        <v>0.987178034344702</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,10 +1329,12 @@
         <v>13</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>85</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>0.996230208</v>
+        <f aca="false">B25+1</f>
+        <v>24</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <f aca="false">D25+$E$3</f>
+        <v>0.986737939748477</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1223,10 +1342,12 @@
         <v>13</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>105</v>
-      </c>
-      <c r="C27" s="0" t="n">
-        <v>0.996093536</v>
+        <f aca="false">B26+1</f>
+        <v>25</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">D26+$E$3</f>
+        <v>0.986297845152252</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1234,10 +1355,12 @@
         <v>13</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>115</v>
-      </c>
-      <c r="C28" s="0" t="n">
-        <v>0.995956647</v>
+        <f aca="false">B27+1</f>
+        <v>26</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <f aca="false">D27+$E$3</f>
+        <v>0.985857750556027</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1245,10 +1368,12 @@
         <v>13</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>0.995682807</v>
+        <f aca="false">B28+1</f>
+        <v>27</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <f aca="false">D28+$E$3</f>
+        <v>0.985417655959802</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1256,10 +1381,12 @@
         <v>13</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>126</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>0.995545644</v>
+        <f aca="false">B29+1</f>
+        <v>28</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">D29+$E$3</f>
+        <v>0.984977561363578</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1267,10 +1394,12 @@
         <v>13</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>138</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>0.99540837</v>
+        <f aca="false">B30+1</f>
+        <v>29</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <f aca="false">D30+$E$3</f>
+        <v>0.984537466767353</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1278,10 +1407,12 @@
         <v>13</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>0.995271021</v>
+        <f aca="false">B31+1</f>
+        <v>30</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <f aca="false">D31+$E$3</f>
+        <v>0.984097372171128</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1289,10 +1420,12 @@
         <v>13</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>175</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <v>0.995133474</v>
+        <f aca="false">B32+1</f>
+        <v>31</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <f aca="false">D32+$E$3</f>
+        <v>0.983657277574903</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,10 +1433,12 @@
         <v>13</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>176</v>
-      </c>
-      <c r="C34" s="0" t="n">
-        <v>0.994995896</v>
+        <f aca="false">B33+1</f>
+        <v>32</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <f aca="false">D33+$E$3</f>
+        <v>0.983217182978678</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1311,10 +1446,12 @@
         <v>13</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>184</v>
-      </c>
-      <c r="C35" s="0" t="n">
-        <v>0.994858202</v>
+        <f aca="false">B34+1</f>
+        <v>33</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <f aca="false">D34+$E$3</f>
+        <v>0.982777088382453</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1322,10 +1459,12 @@
         <v>13</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>194</v>
-      </c>
-      <c r="C36" s="0" t="n">
-        <v>0.994720462</v>
+        <f aca="false">B35+1</f>
+        <v>34</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <f aca="false">D35+$E$3</f>
+        <v>0.982336993786229</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1333,10 +1472,12 @@
         <v>13</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>198</v>
-      </c>
-      <c r="C37" s="0" t="n">
-        <v>0.994582681</v>
+        <f aca="false">B36+1</f>
+        <v>35</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <f aca="false">D36+$E$3</f>
+        <v>0.981896899190004</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1344,10 +1485,15 @@
         <v>13</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>200</v>
+        <f aca="false">B37+1</f>
+        <v>36</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>0.994444769</v>
+        <v>0.981456804593778</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <f aca="false">D37+$E$3</f>
+        <v>0.981456804593779</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1355,10 +1501,12 @@
         <v>13</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>204</v>
-      </c>
-      <c r="C39" s="0" t="n">
-        <v>0.994306855</v>
+        <f aca="false">B38+1</f>
+        <v>37</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <f aca="false">D38+$E$4</f>
+        <v>0.981240082110955</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1366,10 +1514,12 @@
         <v>13</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>220</v>
-      </c>
-      <c r="C40" s="0" t="n">
-        <v>0.994168642</v>
+        <f aca="false">B39+1</f>
+        <v>38</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <f aca="false">D39+$E$4</f>
+        <v>0.981023359628132</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,10 +1527,12 @@
         <v>13</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>222</v>
-      </c>
-      <c r="C41" s="0" t="n">
-        <v>0.993892249</v>
+        <f aca="false">B40+1</f>
+        <v>39</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <f aca="false">D40+$E$4</f>
+        <v>0.980806637145308</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1388,10 +1540,12 @@
         <v>13</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>258</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <v>0.99375392</v>
+        <f aca="false">B41+1</f>
+        <v>40</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <f aca="false">D41+$E$4</f>
+        <v>0.980589914662485</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1399,10 +1553,12 @@
         <v>13</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>273</v>
-      </c>
-      <c r="C43" s="0" t="n">
-        <v>0.993615459</v>
+        <f aca="false">B42+1</f>
+        <v>41</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <f aca="false">D42+$E$4</f>
+        <v>0.980373192179662</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1410,10 +1566,12 @@
         <v>13</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>276</v>
-      </c>
-      <c r="C44" s="0" t="n">
-        <v>0.993476994</v>
+        <f aca="false">B43+1</f>
+        <v>42</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <f aca="false">D43+$E$4</f>
+        <v>0.980156469696838</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1421,10 +1579,12 @@
         <v>13</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>281</v>
-      </c>
-      <c r="C45" s="0" t="n">
-        <v>0.993338462</v>
+        <f aca="false">B44+1</f>
+        <v>43</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <f aca="false">D44+$E$4</f>
+        <v>0.979939747214015</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1432,10 +1592,12 @@
         <v>13</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>283</v>
-      </c>
-      <c r="C46" s="0" t="n">
-        <v>0.993199829</v>
+        <f aca="false">B45+1</f>
+        <v>44</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <f aca="false">D45+$E$4</f>
+        <v>0.979723024731191</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1443,10 +1605,12 @@
         <v>13</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>299</v>
-      </c>
-      <c r="C47" s="0" t="n">
-        <v>0.992922387</v>
+        <f aca="false">B46+1</f>
+        <v>45</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <f aca="false">D46+$E$4</f>
+        <v>0.979506302248368</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1454,10 +1618,12 @@
         <v>13</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>303</v>
-      </c>
-      <c r="C48" s="0" t="n">
-        <v>0.992783605</v>
+        <f aca="false">B47+1</f>
+        <v>46</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <f aca="false">D47+$E$4</f>
+        <v>0.979289579765544</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1465,10 +1631,12 @@
         <v>13</v>
       </c>
       <c r="B49" s="0" t="n">
-        <v>305</v>
-      </c>
-      <c r="C49" s="0" t="n">
-        <v>0.992644781</v>
+        <f aca="false">B48+1</f>
+        <v>47</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <f aca="false">D48+$E$4</f>
+        <v>0.979072857282721</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,10 +1644,12 @@
         <v>13</v>
       </c>
       <c r="B50" s="0" t="n">
-        <v>320</v>
-      </c>
-      <c r="C50" s="0" t="n">
-        <v>0.992367043</v>
+        <f aca="false">B49+1</f>
+        <v>48</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <f aca="false">D49+$E$4</f>
+        <v>0.978856134799897</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,10 +1657,12 @@
         <v>13</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>323</v>
-      </c>
-      <c r="C51" s="0" t="n">
-        <v>0.992088988</v>
+        <f aca="false">B50+1</f>
+        <v>49</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <f aca="false">D50+$E$4</f>
+        <v>0.978639412317074</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1498,10 +1670,12 @@
         <v>13</v>
       </c>
       <c r="B52" s="0" t="n">
-        <v>328</v>
-      </c>
-      <c r="C52" s="0" t="n">
-        <v>0.991949785</v>
+        <f aca="false">B51+1</f>
+        <v>50</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <f aca="false">D51+$E$4</f>
+        <v>0.978422689834251</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,10 +1683,12 @@
         <v>13</v>
       </c>
       <c r="B53" s="0" t="n">
-        <v>332</v>
-      </c>
-      <c r="C53" s="0" t="n">
-        <v>0.991810561</v>
+        <f aca="false">B52+1</f>
+        <v>51</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <f aca="false">D52+$E$4</f>
+        <v>0.978205967351427</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1520,10 +1696,12 @@
         <v>13</v>
       </c>
       <c r="B54" s="0" t="n">
-        <v>335</v>
-      </c>
-      <c r="C54" s="0" t="n">
-        <v>0.991671252</v>
+        <f aca="false">B53+1</f>
+        <v>52</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <f aca="false">D53+$E$4</f>
+        <v>0.977989244868604</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1531,10 +1709,12 @@
         <v>13</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>340</v>
-      </c>
-      <c r="C55" s="0" t="n">
-        <v>0.991531659</v>
+        <f aca="false">B54+1</f>
+        <v>53</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <f aca="false">D54+$E$4</f>
+        <v>0.97777252238578</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,10 +1722,12 @@
         <v>13</v>
       </c>
       <c r="B56" s="0" t="n">
-        <v>342</v>
-      </c>
-      <c r="C56" s="0" t="n">
-        <v>0.99139196</v>
+        <f aca="false">B55+1</f>
+        <v>54</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <f aca="false">D55+$E$4</f>
+        <v>0.977555799902957</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,10 +1735,12 @@
         <v>13</v>
       </c>
       <c r="B57" s="0" t="n">
-        <v>362</v>
-      </c>
-      <c r="C57" s="0" t="n">
-        <v>0.99125142</v>
+        <f aca="false">B56+1</f>
+        <v>55</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <f aca="false">D56+$E$4</f>
+        <v>0.977339077420133</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1564,10 +1748,12 @@
         <v>13</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>364</v>
-      </c>
-      <c r="C58" s="0" t="n">
-        <v>0.991110848</v>
+        <f aca="false">B57+1</f>
+        <v>56</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <f aca="false">D57+$E$4</f>
+        <v>0.97712235493731</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,10 +1761,12 @@
         <v>13</v>
       </c>
       <c r="B59" s="0" t="n">
-        <v>365</v>
-      </c>
-      <c r="C59" s="0" t="n">
-        <v>0.990970235</v>
+        <f aca="false">B58+1</f>
+        <v>57</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <f aca="false">D58+$E$4</f>
+        <v>0.976905632454486</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,10 +1774,12 @@
         <v>13</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>366</v>
-      </c>
-      <c r="C60" s="0" t="n">
-        <v>0.990829556</v>
+        <f aca="false">B59+1</f>
+        <v>58</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <f aca="false">D59+$E$4</f>
+        <v>0.976688909971663</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1597,10 +1787,12 @@
         <v>13</v>
       </c>
       <c r="B61" s="0" t="n">
-        <v>383</v>
-      </c>
-      <c r="C61" s="0" t="n">
-        <v>0.990688689</v>
+        <f aca="false">B60+1</f>
+        <v>59</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <f aca="false">D60+$E$4</f>
+        <v>0.976472187488839</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1608,2201 +1800,1720 @@
         <v>13</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>438</v>
+        <f aca="false">B61+1</f>
+        <v>60</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>0.990547177</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.976255465006015</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <f aca="false">D61+$E$4</f>
+        <v>0.976255465006016</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B63" s="0" t="n">
-        <v>443</v>
-      </c>
-      <c r="C63" s="0" t="n">
-        <v>0.990405599</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B62+1</f>
+        <v>61</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <f aca="false">D62+$E$5</f>
+        <v>0.976075630521065</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>447</v>
-      </c>
-      <c r="C64" s="0" t="n">
-        <v>0.990263988</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B63+1</f>
+        <v>62</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <f aca="false">D63+$E$5</f>
+        <v>0.975895796036114</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>454</v>
-      </c>
-      <c r="C65" s="0" t="n">
-        <v>0.989980736</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B64+1</f>
+        <v>63</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <f aca="false">D64+$E$5</f>
+        <v>0.975715961551163</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>459</v>
-      </c>
-      <c r="C66" s="0" t="n">
-        <v>0.989697111</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B65+1</f>
+        <v>64</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <f aca="false">D65+$E$5</f>
+        <v>0.975536127066212</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>466</v>
-      </c>
-      <c r="C67" s="0" t="n">
-        <v>0.989555246</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B66+1</f>
+        <v>65</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <f aca="false">D66+$E$5</f>
+        <v>0.975356292581261</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>470</v>
-      </c>
-      <c r="C68" s="0" t="n">
-        <v>0.989271474</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B67+1</f>
+        <v>66</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <f aca="false">D67+$E$5</f>
+        <v>0.97517645809631</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>480</v>
-      </c>
-      <c r="C69" s="0" t="n">
-        <v>0.989129428</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B68+1</f>
+        <v>67</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <f aca="false">D68+$E$5</f>
+        <v>0.974996623611358</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B70" s="0" t="n">
-        <v>487</v>
-      </c>
-      <c r="C70" s="0" t="n">
-        <v>0.988987199</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B69+1</f>
+        <v>68</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <f aca="false">D69+$E$5</f>
+        <v>0.974816789126407</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>498</v>
-      </c>
-      <c r="C71" s="0" t="n">
-        <v>0.988844912</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B70+1</f>
+        <v>69</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <f aca="false">D70+$E$5</f>
+        <v>0.974636954641456</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B72" s="0" t="n">
-        <v>506</v>
-      </c>
-      <c r="C72" s="0" t="n">
-        <v>0.98870243</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B71+1</f>
+        <v>70</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <f aca="false">D71+$E$5</f>
+        <v>0.974457120156505</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B73" s="0" t="n">
-        <v>510</v>
-      </c>
-      <c r="C73" s="0" t="n">
-        <v>0.988559726</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B72+1</f>
+        <v>71</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <f aca="false">D72+$E$5</f>
+        <v>0.974277285671554</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B74" s="0" t="n">
-        <v>511</v>
-      </c>
-      <c r="C74" s="0" t="n">
-        <v>0.988274168</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B73+1</f>
+        <v>72</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <f aca="false">D73+$E$5</f>
+        <v>0.974097451186603</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B75" s="0" t="n">
-        <v>531</v>
-      </c>
-      <c r="C75" s="0" t="n">
-        <v>0.988131213</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B74+1</f>
+        <v>73</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <f aca="false">D74+$E$5</f>
+        <v>0.973917616701652</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>551</v>
-      </c>
-      <c r="C76" s="0" t="n">
-        <v>0.987987983</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B75+1</f>
+        <v>74</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <f aca="false">D75+$E$5</f>
+        <v>0.973737782216701</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>554</v>
-      </c>
-      <c r="C77" s="0" t="n">
-        <v>0.987844719</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B76+1</f>
+        <v>75</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <f aca="false">D76+$E$5</f>
+        <v>0.97355794773175</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B78" s="0" t="n">
-        <v>572</v>
-      </c>
-      <c r="C78" s="0" t="n">
-        <v>0.987701337</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B77+1</f>
+        <v>76</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <f aca="false">D77+$E$5</f>
+        <v>0.973378113246799</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B79" s="0" t="n">
-        <v>585</v>
-      </c>
-      <c r="C79" s="0" t="n">
-        <v>0.987557836</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B78+1</f>
+        <v>77</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <f aca="false">D78+$E$5</f>
+        <v>0.973198278761848</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B80" s="0" t="n">
-        <v>589</v>
-      </c>
-      <c r="C80" s="0" t="n">
-        <v>0.987414339</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B79+1</f>
+        <v>78</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <f aca="false">D79+$E$5</f>
+        <v>0.973018444276897</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B81" s="0" t="n">
-        <v>605</v>
-      </c>
-      <c r="C81" s="0" t="n">
-        <v>0.987270751</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B80+1</f>
+        <v>79</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <f aca="false">D80+$E$5</f>
+        <v>0.972838609791946</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>606</v>
-      </c>
-      <c r="C82" s="0" t="n">
-        <v>0.987127125</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B81+1</f>
+        <v>80</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <f aca="false">D81+$E$5</f>
+        <v>0.972658775306995</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B83" s="0" t="n">
-        <v>609</v>
-      </c>
-      <c r="C83" s="0" t="n">
-        <v>0.986983453</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B82+1</f>
+        <v>81</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <f aca="false">D82+$E$5</f>
+        <v>0.972478940822044</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>617</v>
-      </c>
-      <c r="C84" s="0" t="n">
-        <v>0.986839688</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B83+1</f>
+        <v>82</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <f aca="false">D83+$E$5</f>
+        <v>0.972299106337093</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B85" s="0" t="n">
-        <v>624</v>
-      </c>
-      <c r="C85" s="0" t="n">
-        <v>0.986695853</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B84+1</f>
+        <v>83</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <f aca="false">D84+$E$5</f>
+        <v>0.972119271852141</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B86" s="0" t="n">
-        <v>639</v>
+        <f aca="false">B85+1</f>
+        <v>84</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>0.986551904</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0.971939437367188</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <f aca="false">D85+$E$5</f>
+        <v>0.97193943736719</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B87" s="0" t="n">
-        <v>640</v>
-      </c>
-      <c r="C87" s="0" t="n">
-        <v>0.986407929</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B86+1</f>
+        <v>85</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <f aca="false">D86+$E$6</f>
+        <v>0.97178905106516</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B88" s="0" t="n">
-        <v>650</v>
-      </c>
-      <c r="C88" s="0" t="n">
-        <v>0.9862639</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B87+1</f>
+        <v>86</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <f aca="false">D87+$E$6</f>
+        <v>0.97163866476313</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B89" s="0" t="n">
-        <v>652</v>
-      </c>
-      <c r="C89" s="0" t="n">
-        <v>0.986119715</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B88+1</f>
+        <v>87</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <f aca="false">D88+$E$6</f>
+        <v>0.971488278461099</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>671</v>
-      </c>
-      <c r="C90" s="0" t="n">
-        <v>0.985975256</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B89+1</f>
+        <v>88</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <f aca="false">D89+$E$6</f>
+        <v>0.971337892159069</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B91" s="0" t="n">
-        <v>677</v>
-      </c>
-      <c r="C91" s="0" t="n">
-        <v>0.98583076</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B90+1</f>
+        <v>89</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <f aca="false">D90+$E$6</f>
+        <v>0.971187505857039</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>725</v>
-      </c>
-      <c r="C92" s="0" t="n">
-        <v>0.985685176</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B91+1</f>
+        <v>90</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <f aca="false">D91+$E$6</f>
+        <v>0.971037119555008</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>739</v>
-      </c>
-      <c r="C93" s="0" t="n">
-        <v>0.98553932</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B92+1</f>
+        <v>91</v>
+      </c>
+      <c r="D93" s="0" t="n">
+        <f aca="false">D92+$E$6</f>
+        <v>0.970886733252978</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>761</v>
-      </c>
-      <c r="C94" s="0" t="n">
-        <v>0.985393256</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B93+1</f>
+        <v>92</v>
+      </c>
+      <c r="D94" s="0" t="n">
+        <f aca="false">D93+$E$6</f>
+        <v>0.970736346950948</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B95" s="0" t="n">
-        <v>768</v>
-      </c>
-      <c r="C95" s="0" t="n">
-        <v>0.985247195</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B94+1</f>
+        <v>93</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <f aca="false">D94+$E$6</f>
+        <v>0.970585960648917</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B96" s="0" t="n">
-        <v>769</v>
-      </c>
-      <c r="C96" s="0" t="n">
-        <v>0.985101096</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B95+1</f>
+        <v>94</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <f aca="false">D95+$E$6</f>
+        <v>0.970435574346887</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B97" s="0" t="n">
-        <v>783</v>
-      </c>
-      <c r="C97" s="0" t="n">
-        <v>0.984954956</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B96+1</f>
+        <v>95</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <f aca="false">D96+$E$6</f>
+        <v>0.970285188044856</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B98" s="0" t="n">
-        <v>799</v>
-      </c>
-      <c r="C98" s="0" t="n">
-        <v>0.984808197</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B97+1</f>
+        <v>96</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <f aca="false">D97+$E$6</f>
+        <v>0.970134801742826</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>803</v>
-      </c>
-      <c r="C99" s="0" t="n">
-        <v>0.984661405</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B98+1</f>
+        <v>97</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <f aca="false">D98+$E$6</f>
+        <v>0.969984415440796</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B100" s="0" t="n">
-        <v>833</v>
-      </c>
-      <c r="C100" s="0" t="n">
-        <v>0.984514449</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B99+1</f>
+        <v>98</v>
+      </c>
+      <c r="D100" s="0" t="n">
+        <f aca="false">D99+$E$6</f>
+        <v>0.969834029138765</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>859</v>
-      </c>
-      <c r="C101" s="0" t="n">
-        <v>0.984367391</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B100+1</f>
+        <v>99</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <f aca="false">D100+$E$6</f>
+        <v>0.969683642836735</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B102" s="0" t="n">
-        <v>870</v>
-      </c>
-      <c r="C102" s="0" t="n">
-        <v>0.984220161</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B101+1</f>
+        <v>100</v>
+      </c>
+      <c r="D102" s="0" t="n">
+        <f aca="false">D101+$E$6</f>
+        <v>0.969533256534705</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>887</v>
-      </c>
-      <c r="C103" s="0" t="n">
-        <v>0.984072664</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B102+1</f>
+        <v>101</v>
+      </c>
+      <c r="D103" s="0" t="n">
+        <f aca="false">D102+$E$6</f>
+        <v>0.969382870232674</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B104" s="0" t="n">
-        <v>888</v>
-      </c>
-      <c r="C104" s="0" t="n">
-        <v>0.983925121</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B103+1</f>
+        <v>102</v>
+      </c>
+      <c r="D104" s="0" t="n">
+        <f aca="false">D103+$E$6</f>
+        <v>0.969232483930644</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>890</v>
-      </c>
-      <c r="C105" s="0" t="n">
-        <v>0.98377753</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B104+1</f>
+        <v>103</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <f aca="false">D104+$E$6</f>
+        <v>0.969082097628614</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>892</v>
-      </c>
-      <c r="C106" s="0" t="n">
-        <v>0.983629939</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B105+1</f>
+        <v>104</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <f aca="false">D105+$E$6</f>
+        <v>0.968931711326583</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B107" s="0" t="n">
-        <v>906</v>
-      </c>
-      <c r="C107" s="0" t="n">
-        <v>0.983482223</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B106+1</f>
+        <v>105</v>
+      </c>
+      <c r="D107" s="0" t="n">
+        <f aca="false">D106+$E$6</f>
+        <v>0.968781325024553</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>915</v>
-      </c>
-      <c r="C108" s="0" t="n">
-        <v>0.983334403</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B107+1</f>
+        <v>106</v>
+      </c>
+      <c r="D108" s="0" t="n">
+        <f aca="false">D107+$E$6</f>
+        <v>0.968630938722523</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>923</v>
-      </c>
-      <c r="C109" s="0" t="n">
-        <v>0.983186464</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B108+1</f>
+        <v>107</v>
+      </c>
+      <c r="D109" s="0" t="n">
+        <f aca="false">D108+$E$6</f>
+        <v>0.968480552420492</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B110" s="0" t="n">
-        <v>941</v>
-      </c>
-      <c r="C110" s="0" t="n">
-        <v>0.983038334</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B109+1</f>
+        <v>108</v>
+      </c>
+      <c r="D110" s="0" t="n">
+        <f aca="false">D109+$E$6</f>
+        <v>0.968330166118462</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>942</v>
-      </c>
-      <c r="C111" s="0" t="n">
-        <v>0.982890126</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B110+1</f>
+        <v>109</v>
+      </c>
+      <c r="D111" s="0" t="n">
+        <f aca="false">D110+$E$6</f>
+        <v>0.968179779816432</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>947</v>
-      </c>
-      <c r="C112" s="0" t="n">
-        <v>0.982741897</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B111+1</f>
+        <v>110</v>
+      </c>
+      <c r="D112" s="0" t="n">
+        <f aca="false">D111+$E$6</f>
+        <v>0.968029393514401</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>973</v>
-      </c>
-      <c r="C113" s="0" t="n">
-        <v>0.982593397</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B112+1</f>
+        <v>111</v>
+      </c>
+      <c r="D113" s="0" t="n">
+        <f aca="false">D112+$E$6</f>
+        <v>0.967879007212371</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B114" s="0" t="n">
-        <v>975</v>
-      </c>
-      <c r="C114" s="0" t="n">
-        <v>0.982444858</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B113+1</f>
+        <v>112</v>
+      </c>
+      <c r="D114" s="0" t="n">
+        <f aca="false">D113+$E$6</f>
+        <v>0.967728620910341</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>986</v>
-      </c>
-      <c r="C115" s="0" t="n">
-        <v>0.982296221</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B114+1</f>
+        <v>113</v>
+      </c>
+      <c r="D115" s="0" t="n">
+        <f aca="false">D114+$E$6</f>
+        <v>0.96757823460831</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B116" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C116" s="0" t="n">
-        <v>0.982147162</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B115+1</f>
+        <v>114</v>
+      </c>
+      <c r="D116" s="0" t="n">
+        <f aca="false">D115+$E$6</f>
+        <v>0.96742784830628</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>1007</v>
-      </c>
-      <c r="C117" s="0" t="n">
-        <v>0.981997831</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B116+1</f>
+        <v>115</v>
+      </c>
+      <c r="D117" s="0" t="n">
+        <f aca="false">D116+$E$6</f>
+        <v>0.96727746200425</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B118" s="0" t="n">
-        <v>1015</v>
-      </c>
-      <c r="C118" s="0" t="n">
-        <v>0.981848405</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B117+1</f>
+        <v>116</v>
+      </c>
+      <c r="D118" s="0" t="n">
+        <f aca="false">D117+$E$6</f>
+        <v>0.967127075702219</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B119" s="0" t="n">
-        <v>1020</v>
-      </c>
-      <c r="C119" s="0" t="n">
-        <v>0.981698917</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B118+1</f>
+        <v>117</v>
+      </c>
+      <c r="D119" s="0" t="n">
+        <f aca="false">D118+$E$6</f>
+        <v>0.966976689400189</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B120" s="0" t="n">
-        <v>1023</v>
-      </c>
-      <c r="C120" s="0" t="n">
-        <v>0.981549357</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B119+1</f>
+        <v>118</v>
+      </c>
+      <c r="D120" s="0" t="n">
+        <f aca="false">D119+$E$6</f>
+        <v>0.966826303098159</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>1047</v>
-      </c>
-      <c r="C121" s="0" t="n">
-        <v>0.981399597</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B120+1</f>
+        <v>119</v>
+      </c>
+      <c r="D121" s="0" t="n">
+        <f aca="false">D120+$E$6</f>
+        <v>0.966675916796128</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B122" s="0" t="n">
-        <v>1048</v>
+        <f aca="false">B121+1</f>
+        <v>120</v>
       </c>
       <c r="C122" s="0" t="n">
-        <v>0.981249798</v>
+        <v>0.966525530494094</v>
+      </c>
+      <c r="D122" s="0" t="n">
+        <f aca="false">D121+$E$6</f>
+        <v>0.966525530494098</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B123" s="0" t="n">
-        <v>1053</v>
-      </c>
-      <c r="C123" s="0" t="n">
-        <v>0.981099953</v>
-      </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B124" s="0" t="n">
-        <v>1055</v>
-      </c>
-      <c r="C124" s="0" t="n">
-        <v>0.980949776</v>
-      </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B125" s="0" t="n">
-        <v>1056</v>
-      </c>
-      <c r="C125" s="0" t="n">
-        <v>0.980799446</v>
-      </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B126" s="0" t="n">
-        <v>1060</v>
-      </c>
-      <c r="C126" s="0" t="n">
-        <v>0.980648914</v>
-      </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B127" s="0" t="n">
-        <v>1069</v>
-      </c>
-      <c r="C127" s="0" t="n">
-        <v>0.980497989</v>
-      </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B128" s="0" t="n">
-        <v>1092</v>
-      </c>
-      <c r="C128" s="0" t="n">
-        <v>0.980346538</v>
-      </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B129" s="0" t="n">
-        <v>1100</v>
-      </c>
-      <c r="C129" s="0" t="n">
-        <v>0.980194802</v>
-      </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B130" s="0" t="n">
-        <v>1101</v>
-      </c>
-      <c r="C130" s="0" t="n">
-        <v>0.980043002</v>
-      </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B131" s="0" t="n">
-        <v>1118</v>
-      </c>
-      <c r="C131" s="0" t="n">
-        <v>0.97989083</v>
-      </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B132" s="0" t="n">
-        <v>1121</v>
-      </c>
-      <c r="C132" s="0" t="n">
-        <v>0.97973838</v>
-      </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B133" s="0" t="n">
-        <v>1128</v>
-      </c>
-      <c r="C133" s="0" t="n">
-        <v>0.979585755</v>
-      </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B134" s="0" t="n">
-        <v>1131</v>
-      </c>
-      <c r="C134" s="0" t="n">
-        <v>0.979432924</v>
-      </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B135" s="0" t="n">
-        <v>1140</v>
-      </c>
-      <c r="C135" s="0" t="n">
-        <v>0.979279878</v>
-      </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B136" s="0" t="n">
-        <v>1145</v>
-      </c>
-      <c r="C136" s="0" t="n">
-        <v>0.979126615</v>
-      </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B137" s="0" t="n">
-        <v>1151</v>
-      </c>
-      <c r="C137" s="0" t="n">
-        <v>0.978973338</v>
-      </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B138" s="0" t="n">
-        <v>1152</v>
-      </c>
-      <c r="C138" s="0" t="n">
-        <v>0.978819903</v>
-      </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B139" s="0" t="n">
-        <v>1154</v>
-      </c>
-      <c r="C139" s="0" t="n">
-        <v>0.978666466</v>
-      </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B140" s="0" t="n">
-        <v>1159</v>
-      </c>
-      <c r="C140" s="0" t="n">
-        <v>0.978512738</v>
-      </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B141" s="0" t="n">
-        <v>1164</v>
-      </c>
-      <c r="C141" s="0" t="n">
-        <v>0.978358983</v>
-      </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B142" s="0" t="n">
-        <v>1169</v>
-      </c>
-      <c r="C142" s="0" t="n">
-        <v>0.978205078</v>
-      </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B143" s="0" t="n">
-        <v>1171</v>
-      </c>
-      <c r="C143" s="0" t="n">
-        <v>0.978051155</v>
-      </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B144" s="0" t="n">
-        <v>1178</v>
-      </c>
-      <c r="C144" s="0" t="n">
-        <v>0.9778972</v>
-      </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B145" s="0" t="n">
-        <v>1182</v>
-      </c>
-      <c r="C145" s="0" t="n">
-        <v>0.977743173</v>
-      </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B146" s="0" t="n">
-        <v>1200</v>
-      </c>
-      <c r="C146" s="0" t="n">
-        <v>0.977588964</v>
-      </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B147" s="0" t="n">
-        <v>1201</v>
-      </c>
-      <c r="C147" s="0" t="n">
-        <v>0.977434737</v>
-      </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B148" s="0" t="n">
-        <v>1204</v>
-      </c>
-      <c r="C148" s="0" t="n">
-        <v>0.9772805</v>
-      </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B149" s="0" t="n">
-        <v>1211</v>
-      </c>
-      <c r="C149" s="0" t="n">
-        <v>0.977125801</v>
-      </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B150" s="0" t="n">
-        <v>1212</v>
-      </c>
-      <c r="C150" s="0" t="n">
-        <v>0.976970998</v>
-      </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B151" s="0" t="n">
-        <v>1215</v>
-      </c>
-      <c r="C151" s="0" t="n">
-        <v>0.976661066</v>
-      </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B152" s="0" t="n">
-        <v>1224</v>
-      </c>
-      <c r="C152" s="0" t="n">
-        <v>0.976505956</v>
-      </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B153" s="0" t="n">
-        <v>1239</v>
-      </c>
-      <c r="C153" s="0" t="n">
-        <v>0.976350773</v>
-      </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B154" s="0" t="n">
-        <v>1246</v>
-      </c>
-      <c r="C154" s="0" t="n">
-        <v>0.976195493</v>
-      </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B155" s="0" t="n">
-        <v>1252</v>
-      </c>
-      <c r="C155" s="0" t="n">
-        <v>0.976040147</v>
-      </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B156" s="0" t="n">
-        <v>1272</v>
-      </c>
-      <c r="C156" s="0" t="n">
-        <v>0.975884686</v>
-      </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B157" s="0" t="n">
-        <v>1273</v>
-      </c>
-      <c r="C157" s="0" t="n">
-        <v>0.975729174</v>
-      </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B158" s="0" t="n">
-        <v>1282</v>
-      </c>
-      <c r="C158" s="0" t="n">
-        <v>0.975573422</v>
-      </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B159" s="0" t="n">
-        <v>1286</v>
-      </c>
-      <c r="C159" s="0" t="n">
-        <v>0.97541766</v>
-      </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B160" s="0" t="n">
-        <v>1304</v>
-      </c>
-      <c r="C160" s="0" t="n">
-        <v>0.975261664</v>
-      </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B161" s="0" t="n">
-        <v>1316</v>
-      </c>
-      <c r="C161" s="0" t="n">
-        <v>0.975105482</v>
-      </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B162" s="0" t="n">
-        <v>1319</v>
-      </c>
-      <c r="C162" s="0" t="n">
-        <v>0.974949288</v>
-      </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B163" s="0" t="n">
-        <v>1326</v>
-      </c>
-      <c r="C163" s="0" t="n">
-        <v>0.974792895</v>
-      </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B164" s="0" t="n">
-        <v>1333</v>
-      </c>
-      <c r="C164" s="0" t="n">
-        <v>0.974636484</v>
-      </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B165" s="0" t="n">
-        <v>1359</v>
-      </c>
-      <c r="C165" s="0" t="n">
-        <v>0.974478803</v>
-      </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B166" s="0" t="n">
-        <v>1376</v>
-      </c>
-      <c r="C166" s="0" t="n">
-        <v>0.974162749</v>
-      </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B167" s="0" t="n">
-        <v>1385</v>
-      </c>
-      <c r="C167" s="0" t="n">
-        <v>0.974004598</v>
-      </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B168" s="0" t="n">
-        <v>1386</v>
-      </c>
-      <c r="C168" s="0" t="n">
-        <v>0.973846377</v>
-      </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B169" s="0" t="n">
-        <v>1395</v>
-      </c>
-      <c r="C169" s="0" t="n">
-        <v>0.973528838</v>
-      </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B170" s="0" t="n">
-        <v>1398</v>
-      </c>
-      <c r="C170" s="0" t="n">
-        <v>0.973369821</v>
-      </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B171" s="0" t="n">
-        <v>1399</v>
-      </c>
-      <c r="C171" s="0" t="n">
-        <v>0.973210819</v>
-      </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B172" s="0" t="n">
-        <v>1411</v>
-      </c>
-      <c r="C172" s="0" t="n">
-        <v>0.97305058</v>
-      </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B173" s="0" t="n">
-        <v>1438</v>
-      </c>
-      <c r="C173" s="0" t="n">
-        <v>0.972887539</v>
-      </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B174" s="0" t="n">
-        <v>1485</v>
-      </c>
-      <c r="C174" s="0" t="n">
-        <v>0.9727196</v>
-      </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B175" s="0" t="n">
-        <v>1492</v>
-      </c>
-      <c r="C175" s="0" t="n">
-        <v>0.972550895</v>
-      </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B176" s="0" t="n">
-        <v>1497</v>
-      </c>
-      <c r="C176" s="0" t="n">
-        <v>0.972381981</v>
-      </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B177" s="0" t="n">
-        <v>1500</v>
-      </c>
-      <c r="C177" s="0" t="n">
-        <v>0.972212783</v>
-      </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B178" s="0" t="n">
-        <v>1501</v>
-      </c>
-      <c r="C178" s="0" t="n">
-        <v>0.972043546</v>
-      </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B179" s="0" t="n">
-        <v>1502</v>
-      </c>
-      <c r="C179" s="0" t="n">
-        <v>0.971874043</v>
-      </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B180" s="0" t="n">
-        <v>1506</v>
-      </c>
-      <c r="C180" s="0" t="n">
-        <v>0.971704422</v>
-      </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B181" s="0" t="n">
-        <v>1512</v>
-      </c>
-      <c r="C181" s="0" t="n">
-        <v>0.97153454</v>
-      </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B182" s="0" t="n">
-        <v>1513</v>
-      </c>
-      <c r="C182" s="0" t="n">
-        <v>0.971364606</v>
-      </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B183" s="0" t="n">
-        <v>1519</v>
-      </c>
-      <c r="C183" s="0" t="n">
-        <v>0.971194485</v>
-      </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B184" s="0" t="n">
-        <v>1525</v>
-      </c>
-      <c r="C184" s="0" t="n">
-        <v>0.971024049</v>
-      </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B185" s="0" t="n">
-        <v>1530</v>
-      </c>
-      <c r="C185" s="0" t="n">
-        <v>0.970853397</v>
-      </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B186" s="0" t="n">
-        <v>1531</v>
-      </c>
-      <c r="C186" s="0" t="n">
-        <v>0.970682639</v>
-      </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B187" s="0" t="n">
-        <v>1535</v>
-      </c>
-      <c r="C187" s="0" t="n">
-        <v>0.970511823</v>
-      </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B188" s="0" t="n">
-        <v>1549</v>
-      </c>
-      <c r="C188" s="0" t="n">
-        <v>0.970340659</v>
-      </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B189" s="0" t="n">
-        <v>1553</v>
-      </c>
-      <c r="C189" s="0" t="n">
-        <v>0.969827073</v>
-      </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B190" s="0" t="n">
-        <v>1561</v>
-      </c>
-      <c r="C190" s="0" t="n">
-        <v>0.969655644</v>
-      </c>
     </row>
     <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B191" s="0" t="n">
-        <v>1569</v>
-      </c>
-      <c r="C191" s="0" t="n">
-        <v>0.969484046</v>
-      </c>
     </row>
     <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B192" s="0" t="n">
-        <v>1584</v>
-      </c>
-      <c r="C192" s="0" t="n">
-        <v>0.969312179</v>
-      </c>
     </row>
     <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B193" s="0" t="n">
-        <v>1586</v>
-      </c>
-      <c r="C193" s="0" t="n">
-        <v>0.969140173</v>
-      </c>
     </row>
     <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B194" s="0" t="n">
-        <v>1611</v>
-      </c>
-      <c r="C194" s="0" t="n">
-        <v>0.968967847</v>
-      </c>
     </row>
     <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B195" s="0" t="n">
-        <v>1614</v>
-      </c>
-      <c r="C195" s="0" t="n">
-        <v>0.968795536</v>
-      </c>
     </row>
     <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B196" s="0" t="n">
-        <v>1622</v>
-      </c>
-      <c r="C196" s="0" t="n">
-        <v>0.968623077</v>
-      </c>
     </row>
     <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B197" s="0" t="n">
-        <v>1623</v>
-      </c>
-      <c r="C197" s="0" t="n">
-        <v>0.968450545</v>
-      </c>
     </row>
     <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B198" s="0" t="n">
-        <v>1627</v>
-      </c>
-      <c r="C198" s="0" t="n">
-        <v>0.968277951</v>
-      </c>
     </row>
     <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B199" s="0" t="n">
-        <v>1629</v>
-      </c>
-      <c r="C199" s="0" t="n">
-        <v>0.968105132</v>
-      </c>
     </row>
     <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B200" s="0" t="n">
-        <v>1640</v>
-      </c>
-      <c r="C200" s="0" t="n">
-        <v>0.967932039</v>
-      </c>
     </row>
     <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B201" s="0" t="n">
-        <v>1641</v>
-      </c>
-      <c r="C201" s="0" t="n">
-        <v>0.967758883</v>
-      </c>
     </row>
     <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B202" s="0" t="n">
-        <v>1651</v>
-      </c>
-      <c r="C202" s="0" t="n">
-        <v>0.967585489</v>
-      </c>
     </row>
     <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B203" s="0" t="n">
-        <v>1657</v>
-      </c>
-      <c r="C203" s="0" t="n">
-        <v>0.967411814</v>
-      </c>
     </row>
     <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B204" s="0" t="n">
-        <v>1673</v>
-      </c>
-      <c r="C204" s="0" t="n">
-        <v>0.967237442</v>
-      </c>
     </row>
     <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B205" s="0" t="n">
-        <v>1678</v>
-      </c>
-      <c r="C205" s="0" t="n">
-        <v>0.967062892</v>
-      </c>
     </row>
     <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B206" s="0" t="n">
-        <v>1680</v>
-      </c>
-      <c r="C206" s="0" t="n">
-        <v>0.966888008</v>
-      </c>
     </row>
     <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B207" s="0" t="n">
-        <v>1681</v>
-      </c>
-      <c r="C207" s="0" t="n">
-        <v>0.966712966</v>
-      </c>
     </row>
     <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B208" s="0" t="n">
-        <v>1688</v>
-      </c>
-      <c r="C208" s="0" t="n">
-        <v>0.96636253</v>
-      </c>
     </row>
     <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B209" s="0" t="n">
-        <v>1697</v>
-      </c>
-      <c r="C209" s="0" t="n">
-        <v>0.966186637</v>
-      </c>
     </row>
     <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B210" s="0" t="n">
-        <v>1714</v>
-      </c>
-      <c r="C210" s="0" t="n">
-        <v>0.96600963</v>
-      </c>
     </row>
     <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B211" s="0" t="n">
-        <v>1716</v>
-      </c>
-      <c r="C211" s="0" t="n">
-        <v>0.965832502</v>
-      </c>
     </row>
     <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B212" s="0" t="n">
-        <v>1748</v>
-      </c>
-      <c r="C212" s="0" t="n">
-        <v>0.96565236</v>
-      </c>
     </row>
     <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B213" s="0" t="n">
-        <v>1773</v>
-      </c>
-      <c r="C213" s="0" t="n">
-        <v>0.965469051</v>
-      </c>
     </row>
     <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B214" s="0" t="n">
-        <v>1777</v>
-      </c>
-      <c r="C214" s="0" t="n">
-        <v>0.965284744</v>
-      </c>
     </row>
     <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B215" s="0" t="n">
-        <v>1778</v>
-      </c>
-      <c r="C215" s="0" t="n">
-        <v>0.965100089</v>
-      </c>
     </row>
     <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B216" s="0" t="n">
-        <v>1779</v>
-      </c>
-      <c r="C216" s="0" t="n">
-        <v>0.96491499</v>
-      </c>
     </row>
     <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B217" s="0" t="n">
-        <v>1783</v>
-      </c>
-      <c r="C217" s="0" t="n">
-        <v>0.964729075</v>
-      </c>
     </row>
     <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B218" s="0" t="n">
-        <v>1784</v>
-      </c>
-      <c r="C218" s="0" t="n">
-        <v>0.964542997</v>
-      </c>
     </row>
     <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B219" s="0" t="n">
-        <v>1797</v>
-      </c>
-      <c r="C219" s="0" t="n">
-        <v>0.964354064</v>
-      </c>
     </row>
     <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B220" s="0" t="n">
-        <v>1802</v>
-      </c>
-      <c r="C220" s="0" t="n">
-        <v>0.964163795</v>
-      </c>
     </row>
     <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B221" s="0" t="n">
-        <v>1808</v>
-      </c>
-      <c r="C221" s="0" t="n">
-        <v>0.963780374</v>
-      </c>
     </row>
     <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B222" s="0" t="n">
-        <v>1811</v>
-      </c>
-      <c r="C222" s="0" t="n">
-        <v>0.963587463</v>
-      </c>
     </row>
     <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B223" s="0" t="n">
-        <v>1816</v>
-      </c>
-      <c r="C223" s="0" t="n">
-        <v>0.963392695</v>
-      </c>
     </row>
     <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B224" s="0" t="n">
-        <v>1826</v>
-      </c>
-      <c r="C224" s="0" t="n">
-        <v>0.963195586</v>
-      </c>
     </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="10"/>
-      <c r="B225" s="10"/>
-      <c r="C225" s="10"/>
+      <c r="A225" s="11"/>
+      <c r="B225" s="11"/>
+      <c r="C225" s="11"/>
     </row>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="10"/>
-      <c r="B226" s="10"/>
-      <c r="C226" s="10"/>
+      <c r="A226" s="11"/>
+      <c r="B226" s="11"/>
+      <c r="C226" s="11"/>
     </row>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="10"/>
-      <c r="B227" s="10"/>
-      <c r="C227" s="10"/>
+      <c r="A227" s="11"/>
+      <c r="B227" s="11"/>
+      <c r="C227" s="11"/>
     </row>
     <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="10"/>
-      <c r="B228" s="10"/>
-      <c r="C228" s="10"/>
+      <c r="A228" s="11"/>
+      <c r="B228" s="11"/>
+      <c r="C228" s="11"/>
     </row>
     <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="10"/>
-      <c r="B229" s="10"/>
-      <c r="C229" s="10"/>
+      <c r="A229" s="11"/>
+      <c r="B229" s="11"/>
+      <c r="C229" s="11"/>
     </row>
     <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="10"/>
-      <c r="B230" s="10"/>
-      <c r="C230" s="10"/>
+      <c r="A230" s="11"/>
+      <c r="B230" s="11"/>
+      <c r="C230" s="11"/>
     </row>
     <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="10"/>
-      <c r="B231" s="10"/>
-      <c r="C231" s="10"/>
+      <c r="A231" s="11"/>
+      <c r="B231" s="11"/>
+      <c r="C231" s="11"/>
     </row>
     <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="10"/>
-      <c r="B232" s="10"/>
-      <c r="C232" s="10"/>
+      <c r="A232" s="11"/>
+      <c r="B232" s="11"/>
+      <c r="C232" s="11"/>
     </row>
     <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="10"/>
-      <c r="B233" s="10"/>
-      <c r="C233" s="10"/>
+      <c r="A233" s="11"/>
+      <c r="B233" s="11"/>
+      <c r="C233" s="11"/>
     </row>
     <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="10"/>
-      <c r="B234" s="10"/>
-      <c r="C234" s="10"/>
+      <c r="A234" s="11"/>
+      <c r="B234" s="11"/>
+      <c r="C234" s="11"/>
     </row>
     <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="10"/>
-      <c r="B235" s="10"/>
-      <c r="C235" s="10"/>
+      <c r="A235" s="11"/>
+      <c r="B235" s="11"/>
+      <c r="C235" s="11"/>
     </row>
     <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="10"/>
-      <c r="B236" s="10"/>
-      <c r="C236" s="10"/>
+      <c r="A236" s="11"/>
+      <c r="B236" s="11"/>
+      <c r="C236" s="11"/>
     </row>
     <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="10"/>
-      <c r="B237" s="10"/>
-      <c r="C237" s="10"/>
+      <c r="A237" s="11"/>
+      <c r="B237" s="11"/>
+      <c r="C237" s="11"/>
     </row>
     <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="10"/>
-      <c r="B238" s="10"/>
-      <c r="C238" s="10"/>
+      <c r="A238" s="11"/>
+      <c r="B238" s="11"/>
+      <c r="C238" s="11"/>
     </row>
     <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="10"/>
-      <c r="B239" s="10"/>
-      <c r="C239" s="10"/>
+      <c r="A239" s="11"/>
+      <c r="B239" s="11"/>
+      <c r="C239" s="11"/>
     </row>
     <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="10"/>
-      <c r="B240" s="10"/>
-      <c r="C240" s="10"/>
+      <c r="A240" s="11"/>
+      <c r="B240" s="11"/>
+      <c r="C240" s="11"/>
     </row>
     <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="10"/>
-      <c r="B241" s="10"/>
-      <c r="C241" s="10"/>
+      <c r="A241" s="11"/>
+      <c r="B241" s="11"/>
+      <c r="C241" s="11"/>
     </row>
     <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="10"/>
-      <c r="B242" s="10"/>
-      <c r="C242" s="10"/>
+      <c r="A242" s="11"/>
+      <c r="B242" s="11"/>
+      <c r="C242" s="11"/>
     </row>
     <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="10"/>
-      <c r="B243" s="10"/>
-      <c r="C243" s="10"/>
+      <c r="A243" s="11"/>
+      <c r="B243" s="11"/>
+      <c r="C243" s="11"/>
     </row>
     <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="10"/>
-      <c r="B244" s="10"/>
-      <c r="C244" s="10"/>
+      <c r="A244" s="11"/>
+      <c r="B244" s="11"/>
+      <c r="C244" s="11"/>
     </row>
     <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="10"/>
-      <c r="B245" s="10"/>
-      <c r="C245" s="10"/>
+      <c r="A245" s="11"/>
+      <c r="B245" s="11"/>
+      <c r="C245" s="11"/>
     </row>
     <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="10"/>
-      <c r="B246" s="10"/>
-      <c r="C246" s="10"/>
+      <c r="A246" s="11"/>
+      <c r="B246" s="11"/>
+      <c r="C246" s="11"/>
     </row>
     <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="10"/>
-      <c r="B247" s="10"/>
-      <c r="C247" s="10"/>
+      <c r="A247" s="11"/>
+      <c r="B247" s="11"/>
+      <c r="C247" s="11"/>
     </row>
     <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="10"/>
-      <c r="B248" s="10"/>
-      <c r="C248" s="10"/>
+      <c r="A248" s="11"/>
+      <c r="B248" s="11"/>
+      <c r="C248" s="11"/>
     </row>
     <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="10"/>
-      <c r="B249" s="10"/>
-      <c r="C249" s="10"/>
+      <c r="A249" s="11"/>
+      <c r="B249" s="11"/>
+      <c r="C249" s="11"/>
     </row>
     <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="10"/>
-      <c r="B250" s="10"/>
-      <c r="C250" s="10"/>
+      <c r="A250" s="11"/>
+      <c r="B250" s="11"/>
+      <c r="C250" s="11"/>
     </row>
     <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="10"/>
-      <c r="B251" s="10"/>
-      <c r="C251" s="10"/>
+      <c r="A251" s="11"/>
+      <c r="B251" s="11"/>
+      <c r="C251" s="11"/>
     </row>
     <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="10"/>
-      <c r="B252" s="10"/>
-      <c r="C252" s="10"/>
+      <c r="A252" s="11"/>
+      <c r="B252" s="11"/>
+      <c r="C252" s="11"/>
     </row>
     <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="10"/>
-      <c r="B253" s="10"/>
-      <c r="C253" s="10"/>
+      <c r="A253" s="11"/>
+      <c r="B253" s="11"/>
+      <c r="C253" s="11"/>
     </row>
     <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="10"/>
-      <c r="B254" s="10"/>
-      <c r="C254" s="10"/>
+      <c r="A254" s="11"/>
+      <c r="B254" s="11"/>
+      <c r="C254" s="11"/>
     </row>
     <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="10"/>
-      <c r="B255" s="10"/>
-      <c r="C255" s="10"/>
+      <c r="A255" s="11"/>
+      <c r="B255" s="11"/>
+      <c r="C255" s="11"/>
     </row>
     <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="10"/>
-      <c r="B256" s="10"/>
-      <c r="C256" s="10"/>
+      <c r="A256" s="11"/>
+      <c r="B256" s="11"/>
+      <c r="C256" s="11"/>
     </row>
     <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="10"/>
-      <c r="B257" s="10"/>
-      <c r="C257" s="10"/>
+      <c r="A257" s="11"/>
+      <c r="B257" s="11"/>
+      <c r="C257" s="11"/>
     </row>
     <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="10"/>
-      <c r="B258" s="10"/>
-      <c r="C258" s="10"/>
+      <c r="A258" s="11"/>
+      <c r="B258" s="11"/>
+      <c r="C258" s="11"/>
     </row>
     <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="10"/>
-      <c r="B259" s="10"/>
-      <c r="C259" s="10"/>
+      <c r="A259" s="11"/>
+      <c r="B259" s="11"/>
+      <c r="C259" s="11"/>
     </row>
     <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="10"/>
-      <c r="B260" s="10"/>
-      <c r="C260" s="10"/>
+      <c r="A260" s="11"/>
+      <c r="B260" s="11"/>
+      <c r="C260" s="11"/>
     </row>
     <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="10"/>
-      <c r="B261" s="10"/>
-      <c r="C261" s="10"/>
+      <c r="A261" s="11"/>
+      <c r="B261" s="11"/>
+      <c r="C261" s="11"/>
     </row>
     <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="10"/>
-      <c r="B262" s="10"/>
-      <c r="C262" s="10"/>
+      <c r="A262" s="11"/>
+      <c r="B262" s="11"/>
+      <c r="C262" s="11"/>
     </row>
     <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="10"/>
-      <c r="B263" s="10"/>
-      <c r="C263" s="10"/>
+      <c r="A263" s="11"/>
+      <c r="B263" s="11"/>
+      <c r="C263" s="11"/>
     </row>
     <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="10"/>
-      <c r="B264" s="10"/>
-      <c r="C264" s="10"/>
+      <c r="A264" s="11"/>
+      <c r="B264" s="11"/>
+      <c r="C264" s="11"/>
     </row>
     <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="10"/>
-      <c r="B265" s="10"/>
-      <c r="C265" s="10"/>
+      <c r="A265" s="11"/>
+      <c r="B265" s="11"/>
+      <c r="C265" s="11"/>
     </row>
     <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="10"/>
-      <c r="B266" s="10"/>
-      <c r="C266" s="10"/>
+      <c r="A266" s="11"/>
+      <c r="B266" s="11"/>
+      <c r="C266" s="11"/>
     </row>
     <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="10"/>
-      <c r="B267" s="10"/>
-      <c r="C267" s="10"/>
+      <c r="A267" s="11"/>
+      <c r="B267" s="11"/>
+      <c r="C267" s="11"/>
     </row>
     <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="10"/>
-      <c r="B268" s="10"/>
-      <c r="C268" s="10"/>
+      <c r="A268" s="11"/>
+      <c r="B268" s="11"/>
+      <c r="C268" s="11"/>
     </row>
     <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="10"/>
-      <c r="B269" s="10"/>
-      <c r="C269" s="10"/>
+      <c r="A269" s="11"/>
+      <c r="B269" s="11"/>
+      <c r="C269" s="11"/>
     </row>
     <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="10"/>
-      <c r="B270" s="10"/>
-      <c r="C270" s="10"/>
+      <c r="A270" s="11"/>
+      <c r="B270" s="11"/>
+      <c r="C270" s="11"/>
     </row>
     <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="10"/>
-      <c r="B271" s="10"/>
-      <c r="C271" s="10"/>
+      <c r="A271" s="11"/>
+      <c r="B271" s="11"/>
+      <c r="C271" s="11"/>
     </row>
     <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="10"/>
-      <c r="B272" s="10"/>
-      <c r="C272" s="10"/>
+      <c r="A272" s="11"/>
+      <c r="B272" s="11"/>
+      <c r="C272" s="11"/>
     </row>
     <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="10"/>
-      <c r="B273" s="10"/>
-      <c r="C273" s="10"/>
+      <c r="A273" s="11"/>
+      <c r="B273" s="11"/>
+      <c r="C273" s="11"/>
     </row>
     <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="10"/>
-      <c r="B274" s="10"/>
-      <c r="C274" s="10"/>
+      <c r="A274" s="11"/>
+      <c r="B274" s="11"/>
+      <c r="C274" s="11"/>
     </row>
     <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="10"/>
-      <c r="B275" s="10"/>
-      <c r="C275" s="10"/>
+      <c r="A275" s="11"/>
+      <c r="B275" s="11"/>
+      <c r="C275" s="11"/>
     </row>
     <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="10"/>
-      <c r="B276" s="10"/>
-      <c r="C276" s="10"/>
+      <c r="A276" s="11"/>
+      <c r="B276" s="11"/>
+      <c r="C276" s="11"/>
     </row>
     <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="10"/>
-      <c r="B277" s="10"/>
-      <c r="C277" s="10"/>
+      <c r="A277" s="11"/>
+      <c r="B277" s="11"/>
+      <c r="C277" s="11"/>
     </row>
     <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="10"/>
-      <c r="B278" s="10"/>
-      <c r="C278" s="10"/>
+      <c r="A278" s="11"/>
+      <c r="B278" s="11"/>
+      <c r="C278" s="11"/>
     </row>
     <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="10"/>
-      <c r="B279" s="10"/>
-      <c r="C279" s="10"/>
+      <c r="A279" s="11"/>
+      <c r="B279" s="11"/>
+      <c r="C279" s="11"/>
     </row>
     <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="10"/>
-      <c r="B280" s="10"/>
-      <c r="C280" s="10"/>
+      <c r="A280" s="11"/>
+      <c r="B280" s="11"/>
+      <c r="C280" s="11"/>
     </row>
     <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="10"/>
-      <c r="B281" s="10"/>
-      <c r="C281" s="10"/>
+      <c r="A281" s="11"/>
+      <c r="B281" s="11"/>
+      <c r="C281" s="11"/>
     </row>
     <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="10"/>
-      <c r="B282" s="10"/>
-      <c r="C282" s="10"/>
+      <c r="A282" s="11"/>
+      <c r="B282" s="11"/>
+      <c r="C282" s="11"/>
     </row>
     <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="10"/>
-      <c r="B283" s="10"/>
-      <c r="C283" s="10"/>
+      <c r="A283" s="11"/>
+      <c r="B283" s="11"/>
+      <c r="C283" s="11"/>
     </row>
     <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="10"/>
-      <c r="B284" s="10"/>
-      <c r="C284" s="10"/>
+      <c r="A284" s="11"/>
+      <c r="B284" s="11"/>
+      <c r="C284" s="11"/>
     </row>
     <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="10"/>
-      <c r="B285" s="10"/>
-      <c r="C285" s="10"/>
+      <c r="A285" s="11"/>
+      <c r="B285" s="11"/>
+      <c r="C285" s="11"/>
     </row>
     <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="10"/>
-      <c r="B286" s="10"/>
-      <c r="C286" s="10"/>
+      <c r="A286" s="11"/>
+      <c r="B286" s="11"/>
+      <c r="C286" s="11"/>
     </row>
     <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="10"/>
-      <c r="B287" s="10"/>
-      <c r="C287" s="10"/>
+      <c r="A287" s="11"/>
+      <c r="B287" s="11"/>
+      <c r="C287" s="11"/>
     </row>
     <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="10"/>
-      <c r="B288" s="10"/>
-      <c r="C288" s="10"/>
+      <c r="A288" s="11"/>
+      <c r="B288" s="11"/>
+      <c r="C288" s="11"/>
     </row>
     <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="10"/>
-      <c r="B289" s="10"/>
-      <c r="C289" s="10"/>
+      <c r="A289" s="11"/>
+      <c r="B289" s="11"/>
+      <c r="C289" s="11"/>
     </row>
     <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="10"/>
-      <c r="B290" s="10"/>
-      <c r="C290" s="10"/>
+      <c r="A290" s="11"/>
+      <c r="B290" s="11"/>
+      <c r="C290" s="11"/>
     </row>
     <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="10"/>
-      <c r="B291" s="10"/>
-      <c r="C291" s="10"/>
+      <c r="A291" s="11"/>
+      <c r="B291" s="11"/>
+      <c r="C291" s="11"/>
     </row>
     <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="10"/>
-      <c r="B292" s="10"/>
-      <c r="C292" s="10"/>
+      <c r="A292" s="11"/>
+      <c r="B292" s="11"/>
+      <c r="C292" s="11"/>
     </row>
     <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="10"/>
-      <c r="B293" s="10"/>
-      <c r="C293" s="10"/>
+      <c r="A293" s="11"/>
+      <c r="B293" s="11"/>
+      <c r="C293" s="11"/>
     </row>
     <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="10"/>
-      <c r="B294" s="10"/>
-      <c r="C294" s="10"/>
+      <c r="A294" s="11"/>
+      <c r="B294" s="11"/>
+      <c r="C294" s="11"/>
     </row>
     <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="10"/>
-      <c r="B295" s="10"/>
-      <c r="C295" s="10"/>
+      <c r="A295" s="11"/>
+      <c r="B295" s="11"/>
+      <c r="C295" s="11"/>
     </row>
     <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="10"/>
-      <c r="B296" s="10"/>
-      <c r="C296" s="10"/>
+      <c r="A296" s="11"/>
+      <c r="B296" s="11"/>
+      <c r="C296" s="11"/>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="10"/>
-      <c r="B297" s="10"/>
-      <c r="C297" s="10"/>
+      <c r="A297" s="11"/>
+      <c r="B297" s="11"/>
+      <c r="C297" s="11"/>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="10"/>
-      <c r="B298" s="10"/>
-      <c r="C298" s="10"/>
+      <c r="A298" s="11"/>
+      <c r="B298" s="11"/>
+      <c r="C298" s="11"/>
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="10"/>
-      <c r="B299" s="10"/>
-      <c r="C299" s="10"/>
+      <c r="A299" s="11"/>
+      <c r="B299" s="11"/>
+      <c r="C299" s="11"/>
     </row>
     <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="10"/>
-      <c r="B300" s="10"/>
-      <c r="C300" s="10"/>
+      <c r="A300" s="11"/>
+      <c r="B300" s="11"/>
+      <c r="C300" s="11"/>
     </row>
     <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="10"/>
-      <c r="B301" s="10"/>
-      <c r="C301" s="10"/>
+      <c r="A301" s="11"/>
+      <c r="B301" s="11"/>
+      <c r="C301" s="11"/>
     </row>
     <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="10"/>
-      <c r="B302" s="10"/>
-      <c r="C302" s="10"/>
+      <c r="A302" s="11"/>
+      <c r="B302" s="11"/>
+      <c r="C302" s="11"/>
     </row>
     <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="10"/>
-      <c r="B303" s="10"/>
-      <c r="C303" s="10"/>
+      <c r="A303" s="11"/>
+      <c r="B303" s="11"/>
+      <c r="C303" s="11"/>
     </row>
     <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="10"/>
-      <c r="B304" s="10"/>
-      <c r="C304" s="10"/>
+      <c r="A304" s="11"/>
+      <c r="B304" s="11"/>
+      <c r="C304" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3815,7 +3526,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="D87:D122 C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3825,10 +3536,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -3836,7 +3547,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -3847,7 +3558,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -3858,7 +3569,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -3869,7 +3580,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -3897,12 +3608,12 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="H23" activeCellId="1" sqref="D87:D122 H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.45703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3921,43 +3632,43 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="15" t="s">
         <v>44</v>
       </c>
       <c r="N1" s="0" t="s">
@@ -4153,7 +3864,7 @@
       <c r="F10" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="16" t="s">
         <v>51</v>
       </c>
       <c r="I10" s="0" t="n">
@@ -4263,7 +3974,7 @@
       <c r="F15" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="16" t="s">
         <v>51</v>
       </c>
       <c r="I15" s="0" t="n">
@@ -4322,7 +4033,7 @@
         <v>50</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>80</v>
@@ -4339,7 +4050,7 @@
         <v>82</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>2</v>
@@ -4391,7 +4102,7 @@
         <v>82</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>4</v>
@@ -4414,16 +4125,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="C23" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="D23" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>0</v>
@@ -4432,13 +4143,13 @@
         <v>50</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>90</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N23" s="0" t="n">
         <v>0</v>
@@ -4446,13 +4157,13 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>93</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>0.678</v>
@@ -4464,7 +4175,7 @@
         <v>90</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N24" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
KCP-50 - rework printout
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28020"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C9846A1-898A-4933-8C27-D0DF19B954AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD876AEB-C1A9-4D38-B9B7-7B84A209839E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="5" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="109">
   <si>
     <t>Notes</t>
   </si>
@@ -200,8 +200,11 @@
     <t>:v-radio</t>
   </si>
   <si>
-    <t>[:p    [:p "The pathological stage of a kidney cancer tumour is a measure of its size and how far it has spread. This is determined by assessing cancer tissue removed during surgery."]
-   [:ul                                                                                                                                                                                                           
+    <t>Stage 1a (or pT1a) – the cancer is small (4cm or smaller) and only inside the kidney</t>
+  </si>
+  <si>
+    <t>[:p "The pathological stage of a kidney cancer tumour is a measure of its size and how far it has spread. This is determined by assessing cancer tissue removed during surgery."
+   [:ul
       [:li "Stage 1a (or pT1a) – the cancer is small (4cm or smaller) and only inside the kidney"]
       [:li "Stage 1b (or pT1b) – the cancer is small (between 4cm and 7 cm) and only inside the kidney"]
       [:li "Stage 2a (pT2a) - the cancer is between 7cm and 10cm and only inside the kidney"]
@@ -219,42 +222,63 @@
     <t>pT1b</t>
   </si>
   <si>
+    <t>Stage 1b (or pT1b) – the cancer is small (between 4cm and 7 cm) and only inside the kidney</t>
+  </si>
+  <si>
     <t>:pT2a</t>
   </si>
   <si>
     <t>pT2a</t>
   </si>
   <si>
+    <t>Stage 2a (pT2a) - the cancer is between 7cm and 10cm and only inside the kidney</t>
+  </si>
+  <si>
     <t>:pT2b</t>
   </si>
   <si>
     <t>pT2b</t>
   </si>
   <si>
+    <t>Stage 2b (pT2b) – the cancer is larger than 10cm and only inside the kidney</t>
+  </si>
+  <si>
     <t>:pT3a</t>
   </si>
   <si>
     <t>pT3a</t>
   </si>
   <si>
+    <t>Stage 3a (or pT3a) – the cancer is growing into the fat around the kidney, or into the renal vein</t>
+  </si>
+  <si>
     <t>:pT3b</t>
   </si>
   <si>
     <t>pT3b</t>
   </si>
   <si>
+    <t>Stage 3b (or pT3b) - the cancer is growing into the vena cava in the tummy (abdomen)</t>
+  </si>
+  <si>
     <t>:pT3c</t>
   </si>
   <si>
     <t>pT3c</t>
   </si>
   <si>
+    <t>Stage 3c (or pT3c) - the cancer is growing into the vena cava in the chest, or into the wall of the vena cava.</t>
+  </si>
+  <si>
     <t>:pT4</t>
   </si>
   <si>
     <t>pT4</t>
   </si>
   <si>
+    <t>Stage 4 (or pT4) - the cancer has spread through the capsule that surrounds the kidney. It may have grown into the adrenal gland</t>
+  </si>
+  <si>
     <t>:n-stage</t>
   </si>
   <si>
@@ -267,7 +291,7 @@
     <t>Unknown</t>
   </si>
   <si>
-    <t>[:p  [:p "The regional lymph node status indicates if the cancer has spread to lymph nodes near the kidney. Lymph nodes are a network of glands found throughout the body that drain away waste fluid, waste products and damaged cells. They also fight infections."]                  
+    <t>[:p "The regional lymph node status indicates if the cancer has spread to lymph nodes near the kidney. Lymph nodes are a network of glands found throughout the body that drain away waste fluid, waste products and damaged cells. They also fight infections."
   [:ul
       [:li "Unknown (pNx) – There were no lymph nodes found in the tumour samples removed at the time of surgery"]
       [:li "pN0 – No cancer was detected in any lymph nodes near the tumour"]
@@ -2411,8 +2435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E203"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A122" sqref="A43:A122"/>
+    <sheetView showGridLines="0" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C122" sqref="A2:C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4234,8 +4258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4245,8 +4269,8 @@
     <col min="3" max="3" width="31" style="1" customWidth="1"/>
     <col min="4" max="4" width="43" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="81" style="1" customWidth="1"/>
     <col min="8" max="8" width="116.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="5.21875" style="1" customWidth="1"/>
     <col min="10" max="12" width="14.21875" style="1" customWidth="1"/>
@@ -4318,9 +4342,11 @@
       <c r="F2" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="23"/>
+      <c r="G2" s="58" t="s">
+        <v>51</v>
+      </c>
       <c r="H2" s="57" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I2" s="43">
         <v>50</v>
@@ -4340,25 +4366,26 @@
         <v>46</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E3" s="25">
         <v>1.2430000000000001</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="58"/>
+      <c r="G3" s="58" t="s">
+        <v>55</v>
+      </c>
       <c r="I3" s="25">
         <v>50</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="44">
@@ -4370,25 +4397,26 @@
         <v>46</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" s="25">
         <v>1.6479999999999999</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="58"/>
+      <c r="G4" s="58" t="s">
+        <v>58</v>
+      </c>
       <c r="I4" s="25">
         <v>50</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="44">
@@ -4400,25 +4428,26 @@
         <v>46</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E5" s="25">
         <v>1.6479999999999999</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="58"/>
+      <c r="G5" s="58" t="s">
+        <v>61</v>
+      </c>
       <c r="I5" s="25">
         <v>50</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="44">
@@ -4430,25 +4459,26 @@
         <v>46</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E6" s="25">
         <v>1.8959999999999999</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="58"/>
+      <c r="G6" s="58" t="s">
+        <v>64</v>
+      </c>
       <c r="I6" s="25">
         <v>50</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="9" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="44">
@@ -4460,25 +4490,26 @@
         <v>46</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="9" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E7" s="25">
         <v>2.0139999999999998</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="58"/>
+      <c r="G7" s="58" t="s">
+        <v>67</v>
+      </c>
       <c r="I7" s="25">
         <v>50</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="9" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="44">
@@ -4490,25 +4521,26 @@
         <v>46</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="9" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E8" s="25">
         <v>2.0139999999999998</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="58"/>
+      <c r="G8" s="58" t="s">
+        <v>70</v>
+      </c>
       <c r="I8" s="25">
         <v>50</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="9" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="44">
@@ -4520,17 +4552,19 @@
         <v>46</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="9" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E9" s="25">
         <v>2.0139999999999998</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="H9" s="58"/>
       <c r="I9" s="25">
         <v>50</v>
@@ -4538,7 +4572,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="9" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="44">
@@ -4563,16 +4597,16 @@
     </row>
     <row r="11" spans="1:14" ht="126" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E11" s="25">
         <v>0</v>
@@ -4582,7 +4616,7 @@
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="59" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="I11" s="25">
         <v>60</v>
@@ -4590,7 +4624,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="9" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="44">
@@ -4599,14 +4633,14 @@
     </row>
     <row r="12" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="9" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E12" s="25">
         <v>0</v>
@@ -4622,7 +4656,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="9" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="44">
@@ -4631,14 +4665,14 @@
     </row>
     <row r="13" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="9" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="E13" s="25">
         <v>0.92400000000000004</v>
@@ -4654,7 +4688,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="9" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="44">
@@ -4679,16 +4713,16 @@
     </row>
     <row r="15" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="E15" s="25">
         <v>0</v>
@@ -4698,7 +4732,7 @@
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="60" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="I15" s="25">
         <v>70</v>
@@ -4706,7 +4740,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="9" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="44">
@@ -4715,14 +4749,14 @@
     </row>
     <row r="16" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="9" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E16" s="25">
         <v>0.39300000000000002</v>
@@ -4738,7 +4772,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="9" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="44">
@@ -4763,13 +4797,13 @@
     </row>
     <row r="18" spans="1:14" ht="119.25" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D18" s="25">
         <v>1</v>
@@ -4782,7 +4816,7 @@
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="61" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="I18" s="25">
         <v>80</v>
@@ -4799,10 +4833,10 @@
     </row>
     <row r="19" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="25">
@@ -4831,7 +4865,7 @@
     </row>
     <row r="20" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>34</v>
@@ -4863,10 +4897,10 @@
     </row>
     <row r="21" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="25">
@@ -4911,16 +4945,16 @@
     </row>
     <row r="23" spans="1:14" ht="45.4" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="E23" s="25">
         <v>0</v>
@@ -4930,7 +4964,7 @@
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="61" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="I23" s="25">
         <v>90</v>
@@ -4938,7 +4972,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="9" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="44">
@@ -4947,14 +4981,14 @@
     </row>
     <row r="24" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="9" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E24" s="25">
         <v>0.67800000000000005</v>
@@ -4970,7 +5004,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="9" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="44">
@@ -5008,7 +5042,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" customHeight="1">
       <c r="A1" s="62" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -5018,13 +5052,13 @@
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="45" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>

</xml_diff>

<commit_message>
KCP-39 - update baseline hazard
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27930"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28020"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B355BAC4-70C2-413E-B9B0-0D41B32DA741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C9846A1-898A-4933-8C27-D0DF19B954AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="5" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="101">
   <si>
     <t>Notes</t>
   </si>
@@ -900,9 +900,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -913,6 +910,9 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2411,8 +2411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E203"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A122" sqref="A43:A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2455,11 +2455,10 @@
         <v>13</v>
       </c>
       <c r="B3" s="25">
-        <f>B2+1</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" s="26">
-        <v>0.99875000000000003</v>
+        <v>0.99736231200000003</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -2469,11 +2468,10 @@
         <v>13</v>
       </c>
       <c r="B4" s="25">
-        <f>B3+1</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C4" s="26">
-        <v>0.99750000000000005</v>
+        <v>0.99344794400000003</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
@@ -2483,11 +2481,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="25">
-        <f>B4+1</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C5" s="26">
-        <v>0.99624999999999997</v>
+        <v>0.99094885399999999</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -2497,11 +2494,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="25">
-        <f>B5+1</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C6" s="26">
-        <v>0.995</v>
+        <v>0.98825539500000004</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
@@ -2511,11 +2507,10 @@
         <v>13</v>
       </c>
       <c r="B7" s="25">
-        <f>B6+1</f>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C7" s="26">
-        <v>0.99375000000000002</v>
+        <v>0.98595311900000004</v>
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
@@ -2525,11 +2520,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="25">
-        <f>B7+1</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C8" s="26">
-        <v>0.99250000000000005</v>
+        <v>0.98415284800000002</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -2539,11 +2533,10 @@
         <v>13</v>
       </c>
       <c r="B9" s="25">
-        <f>B8+1</f>
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C9" s="26">
-        <v>0.99124999999999996</v>
+        <v>0.98242645699999998</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
@@ -2553,11 +2546,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="25">
-        <f>B9+1</f>
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C10" s="26">
-        <v>0.99</v>
+        <v>0.98096559699999997</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
@@ -2567,11 +2559,10 @@
         <v>13</v>
       </c>
       <c r="B11" s="25">
-        <f>B10+1</f>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C11" s="26">
-        <v>0.98875000000000002</v>
+        <v>0.97988443700000005</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -2581,11 +2572,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="25">
-        <f>B11+1</f>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C12" s="26">
-        <v>0.98750000000000004</v>
+        <v>0.97877624699999999</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="16"/>
@@ -2595,11 +2585,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="25">
-        <f>B12+1</f>
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C13" s="26">
-        <v>0.98624999999999996</v>
+        <v>0.97810844600000002</v>
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
@@ -2609,11 +2598,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="25">
-        <f>B13+1</f>
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C14" s="26">
-        <v>0.98499999999999999</v>
+        <v>0.976403142</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -2623,11 +2611,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="25">
-        <f>B14+1</f>
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C15" s="26">
-        <v>0.984375</v>
+        <v>0.97556337000000004</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -2637,11 +2624,10 @@
         <v>13</v>
       </c>
       <c r="B16" s="25">
-        <f>B15+1</f>
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="C16" s="26">
-        <v>0.98375000000000001</v>
+        <v>0.974567658</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -2651,11 +2637,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="25">
-        <f>B16+1</f>
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C17" s="26">
-        <v>0.98312500000000003</v>
+        <v>0.97338303199999998</v>
       </c>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -2665,11 +2650,10 @@
         <v>13</v>
       </c>
       <c r="B18" s="25">
-        <f>B17+1</f>
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C18" s="26">
-        <v>0.98250000000000004</v>
+        <v>0.97263131000000003</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
@@ -2679,11 +2663,10 @@
         <v>13</v>
       </c>
       <c r="B19" s="25">
-        <f>B18+1</f>
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C19" s="26">
-        <v>0.98187500000000005</v>
+        <v>0.97173773200000002</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="16"/>
@@ -2693,11 +2676,10 @@
         <v>13</v>
       </c>
       <c r="B20" s="25">
-        <f>B19+1</f>
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="C20" s="26">
-        <v>0.98124999999999996</v>
+        <v>0.97107496000000004</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="16"/>
@@ -2707,11 +2689,10 @@
         <v>13</v>
       </c>
       <c r="B21" s="25">
-        <f>B20+1</f>
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="C21" s="26">
-        <v>0.98062499999999997</v>
+        <v>0.97049154699999995</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="16"/>
@@ -2721,11 +2702,10 @@
         <v>13</v>
       </c>
       <c r="B22" s="25">
-        <f>B21+1</f>
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C22" s="26">
-        <v>0.98</v>
+        <v>0.97019160000000004</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="16"/>
@@ -2735,11 +2715,10 @@
         <v>13</v>
       </c>
       <c r="B23" s="25">
-        <f>B22+1</f>
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="C23" s="26">
-        <v>0.979375</v>
+        <v>0.96972380300000005</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="16"/>
@@ -2749,11 +2728,10 @@
         <v>13</v>
       </c>
       <c r="B24" s="25">
-        <f>B23+1</f>
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C24" s="26">
-        <v>0.97875000000000001</v>
+        <v>0.96880171299999995</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="16"/>
@@ -2763,11 +2741,10 @@
         <v>13</v>
       </c>
       <c r="B25" s="25">
-        <f>B24+1</f>
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="C25" s="26">
-        <v>0.97812500000000002</v>
+        <v>0.96824464899999996</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -2777,11 +2754,10 @@
         <v>13</v>
       </c>
       <c r="B26" s="25">
-        <f>B25+1</f>
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="C26" s="26">
-        <v>0.97750000000000004</v>
+        <v>0.96725684999999995</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="16"/>
@@ -2791,11 +2767,10 @@
         <v>13</v>
       </c>
       <c r="B27" s="25">
-        <f>B26+1</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="C27" s="26">
-        <v>0.97687500000000005</v>
+        <v>0.96673659999999995</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="16"/>
@@ -2805,11 +2780,10 @@
         <v>13</v>
       </c>
       <c r="B28" s="25">
-        <f>B27+1</f>
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="C28" s="26">
-        <v>0.97624999999999995</v>
+        <v>0.96637334200000002</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -2819,11 +2793,10 @@
         <v>13</v>
       </c>
       <c r="B29" s="25">
-        <f>B28+1</f>
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C29" s="26">
-        <v>0.97562499999999996</v>
+        <v>0.965562264</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -2833,11 +2806,10 @@
         <v>13</v>
       </c>
       <c r="B30" s="25">
-        <f>B29+1</f>
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="C30" s="26">
-        <v>0.97499999999999998</v>
+        <v>0.96422562999999994</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
@@ -2847,11 +2819,10 @@
         <v>13</v>
       </c>
       <c r="B31" s="25">
-        <f>B30+1</f>
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="C31" s="26">
-        <v>0.97437499999999999</v>
+        <v>0.96377405800000004</v>
       </c>
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
@@ -2861,11 +2832,10 @@
         <v>13</v>
       </c>
       <c r="B32" s="25">
-        <f>B31+1</f>
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="C32" s="26">
-        <v>0.97375</v>
+        <v>0.963071028</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -2875,11 +2845,10 @@
         <v>13</v>
       </c>
       <c r="B33" s="25">
-        <f>B32+1</f>
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="C33" s="26">
-        <v>0.97312500000000002</v>
+        <v>0.96270893000000002</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
@@ -2889,11 +2858,10 @@
         <v>13</v>
       </c>
       <c r="B34" s="25">
-        <f>B33+1</f>
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="C34" s="26">
-        <v>0.97250000000000003</v>
+        <v>0.96177408499999995</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16"/>
@@ -2903,11 +2871,10 @@
         <v>13</v>
       </c>
       <c r="B35" s="25">
-        <f>B34+1</f>
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="C35" s="26">
-        <v>0.97187500000000004</v>
+        <v>0.96063232399999998</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="16"/>
@@ -2917,11 +2884,10 @@
         <v>13</v>
       </c>
       <c r="B36" s="25">
-        <f>B35+1</f>
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="C36" s="26">
-        <v>0.97124999999999995</v>
+        <v>0.96021503200000002</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16"/>
@@ -2931,11 +2897,10 @@
         <v>13</v>
       </c>
       <c r="B37" s="25">
-        <f>B36+1</f>
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="C37" s="26">
-        <v>0.97062499999999996</v>
+        <v>0.96001898200000002</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="16"/>
@@ -2945,11 +2910,10 @@
         <v>13</v>
       </c>
       <c r="B38" s="25">
-        <f>B37+1</f>
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="C38" s="26">
-        <v>0.97</v>
+        <v>0.95986481800000001</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
@@ -2959,11 +2923,10 @@
         <v>13</v>
       </c>
       <c r="B39" s="25">
-        <f>B38+1</f>
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="C39" s="26">
-        <v>0.96966666666666701</v>
+        <v>0.95861570799999996</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -2973,11 +2936,10 @@
         <v>13</v>
       </c>
       <c r="B40" s="25">
-        <f>B39+1</f>
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="C40" s="26">
-        <v>0.96933333333333305</v>
+        <v>0.95798928100000003</v>
       </c>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -2987,11 +2949,10 @@
         <v>13</v>
       </c>
       <c r="B41" s="25">
-        <f>B40+1</f>
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="C41" s="26">
-        <v>0.96899999999999997</v>
+        <v>0.95751720500000004</v>
       </c>
       <c r="D41" s="16"/>
       <c r="E41" s="16"/>
@@ -3001,1132 +2962,571 @@
         <v>13</v>
       </c>
       <c r="B42" s="25">
-        <f>B41+1</f>
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="C42" s="26">
-        <v>0.96866666666666701</v>
+        <v>0.95665158299999997</v>
       </c>
       <c r="D42" s="16"/>
       <c r="E42" s="16"/>
     </row>
     <row r="43" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A43" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="25">
-        <f>B42+1</f>
-        <v>41</v>
-      </c>
-      <c r="C43" s="26">
-        <v>0.96833333333333305</v>
-      </c>
+      <c r="A43" s="11"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="26"/>
       <c r="D43" s="16"/>
       <c r="E43" s="16"/>
     </row>
     <row r="44" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A44" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" s="25">
-        <f>B43+1</f>
-        <v>42</v>
-      </c>
-      <c r="C44" s="26">
-        <v>0.96799999999999997</v>
-      </c>
+      <c r="A44" s="11"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="26"/>
       <c r="D44" s="16"/>
       <c r="E44" s="16"/>
     </row>
     <row r="45" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A45" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" s="25">
-        <f>B44+1</f>
-        <v>43</v>
-      </c>
-      <c r="C45" s="26">
-        <v>0.96766666666666701</v>
-      </c>
+      <c r="A45" s="11"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="26"/>
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
     </row>
     <row r="46" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A46" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" s="25">
-        <f>B45+1</f>
-        <v>44</v>
-      </c>
-      <c r="C46" s="26">
-        <v>0.96733333333333305</v>
-      </c>
+      <c r="A46" s="11"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="26"/>
       <c r="D46" s="16"/>
       <c r="E46" s="16"/>
     </row>
     <row r="47" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A47" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="25">
-        <f>B46+1</f>
-        <v>45</v>
-      </c>
-      <c r="C47" s="26">
-        <v>0.96699999999999997</v>
-      </c>
+      <c r="A47" s="11"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="26"/>
       <c r="D47" s="16"/>
       <c r="E47" s="16"/>
     </row>
     <row r="48" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A48" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" s="25">
-        <f>B47+1</f>
-        <v>46</v>
-      </c>
-      <c r="C48" s="26">
-        <v>0.96666666666666701</v>
-      </c>
+      <c r="A48" s="11"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="26"/>
       <c r="D48" s="16"/>
       <c r="E48" s="16"/>
     </row>
     <row r="49" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A49" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="25">
-        <f>B48+1</f>
-        <v>47</v>
-      </c>
-      <c r="C49" s="26">
-        <v>0.96633333333333304</v>
-      </c>
+      <c r="A49" s="11"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="26"/>
       <c r="D49" s="16"/>
       <c r="E49" s="16"/>
     </row>
     <row r="50" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A50" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50" s="25">
-        <f>B49+1</f>
-        <v>48</v>
-      </c>
-      <c r="C50" s="26">
-        <v>0.96599999999999997</v>
-      </c>
+      <c r="A50" s="11"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="26"/>
       <c r="D50" s="16"/>
       <c r="E50" s="16"/>
     </row>
     <row r="51" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A51" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="25">
-        <f>B50+1</f>
-        <v>49</v>
-      </c>
-      <c r="C51" s="26">
-        <v>0.96566666666666701</v>
-      </c>
+      <c r="A51" s="11"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="26"/>
       <c r="D51" s="16"/>
       <c r="E51" s="16"/>
     </row>
     <row r="52" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A52" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B52" s="25">
-        <f>B51+1</f>
-        <v>50</v>
-      </c>
-      <c r="C52" s="26">
-        <v>0.96533333333333304</v>
-      </c>
+      <c r="A52" s="11"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="26"/>
       <c r="D52" s="16"/>
       <c r="E52" s="16"/>
     </row>
     <row r="53" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A53" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B53" s="25">
-        <f>B52+1</f>
-        <v>51</v>
-      </c>
-      <c r="C53" s="26">
-        <v>0.96499999999999997</v>
-      </c>
+      <c r="A53" s="11"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="26"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
     </row>
     <row r="54" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A54" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" s="25">
-        <f>B53+1</f>
-        <v>52</v>
-      </c>
-      <c r="C54" s="26">
-        <v>0.96466666666666701</v>
-      </c>
+      <c r="A54" s="11"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="26"/>
       <c r="D54" s="16"/>
       <c r="E54" s="16"/>
     </row>
     <row r="55" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A55" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" s="25">
-        <f>B54+1</f>
-        <v>53</v>
-      </c>
-      <c r="C55" s="26">
-        <v>0.96433333333333304</v>
-      </c>
+      <c r="A55" s="11"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="26"/>
       <c r="D55" s="16"/>
       <c r="E55" s="16"/>
     </row>
     <row r="56" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A56" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B56" s="25">
-        <f>B55+1</f>
-        <v>54</v>
-      </c>
-      <c r="C56" s="26">
-        <v>0.96399999999999997</v>
-      </c>
+      <c r="A56" s="11"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="26"/>
       <c r="D56" s="16"/>
       <c r="E56" s="16"/>
     </row>
     <row r="57" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A57" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B57" s="25">
-        <f>B56+1</f>
-        <v>55</v>
-      </c>
-      <c r="C57" s="26">
-        <v>0.963666666666667</v>
-      </c>
+      <c r="A57" s="11"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="26"/>
       <c r="D57" s="16"/>
       <c r="E57" s="16"/>
     </row>
     <row r="58" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A58" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="25">
-        <f>B57+1</f>
-        <v>56</v>
-      </c>
-      <c r="C58" s="26">
-        <v>0.96333333333333304</v>
-      </c>
+      <c r="A58" s="11"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="26"/>
       <c r="D58" s="16"/>
       <c r="E58" s="16"/>
     </row>
     <row r="59" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A59" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B59" s="25">
-        <f>B58+1</f>
-        <v>57</v>
-      </c>
-      <c r="C59" s="26">
-        <v>0.96299999999999997</v>
-      </c>
+      <c r="A59" s="11"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="26"/>
       <c r="D59" s="16"/>
       <c r="E59" s="16"/>
     </row>
     <row r="60" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A60" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="25">
-        <f>B59+1</f>
-        <v>58</v>
-      </c>
-      <c r="C60" s="26">
-        <v>0.962666666666667</v>
-      </c>
+      <c r="A60" s="11"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="26"/>
       <c r="D60" s="16"/>
       <c r="E60" s="16"/>
     </row>
     <row r="61" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A61" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" s="25">
-        <f>B60+1</f>
-        <v>59</v>
-      </c>
-      <c r="C61" s="26">
-        <v>0.96233333333333304</v>
-      </c>
+      <c r="A61" s="11"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="26"/>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
     </row>
     <row r="62" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A62" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" s="25">
-        <f>B61+1</f>
-        <v>60</v>
-      </c>
-      <c r="C62" s="26">
-        <v>0.96199999999999997</v>
-      </c>
+      <c r="A62" s="11"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="26"/>
       <c r="D62" s="16"/>
       <c r="E62" s="16"/>
     </row>
     <row r="63" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A63" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B63" s="25">
-        <f>B62+1</f>
-        <v>61</v>
-      </c>
-      <c r="C63" s="26">
-        <v>0.96170833333333305</v>
-      </c>
+      <c r="A63" s="11"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="26"/>
       <c r="D63" s="16"/>
       <c r="E63" s="16"/>
     </row>
     <row r="64" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A64" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B64" s="25">
-        <f>B63+1</f>
-        <v>62</v>
-      </c>
-      <c r="C64" s="26">
-        <v>0.96141666666666703</v>
-      </c>
+      <c r="A64" s="11"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="26"/>
       <c r="D64" s="16"/>
       <c r="E64" s="16"/>
     </row>
     <row r="65" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A65" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B65" s="25">
-        <f>B64+1</f>
-        <v>63</v>
-      </c>
-      <c r="C65" s="26">
-        <v>0.96112500000000001</v>
-      </c>
+      <c r="A65" s="11"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="26"/>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
     </row>
     <row r="66" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A66" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B66" s="25">
-        <f>B65+1</f>
-        <v>64</v>
-      </c>
-      <c r="C66" s="26">
-        <v>0.96083333333333298</v>
-      </c>
+      <c r="A66" s="11"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="26"/>
       <c r="D66" s="16"/>
       <c r="E66" s="16"/>
     </row>
     <row r="67" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A67" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B67" s="25">
-        <f>B66+1</f>
-        <v>65</v>
-      </c>
-      <c r="C67" s="26">
-        <v>0.96054166666666696</v>
-      </c>
+      <c r="A67" s="11"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="26"/>
       <c r="D67" s="16"/>
       <c r="E67" s="16"/>
     </row>
     <row r="68" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A68" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B68" s="25">
-        <f>B67+1</f>
-        <v>66</v>
-      </c>
-      <c r="C68" s="26">
-        <v>0.96025000000000005</v>
-      </c>
+      <c r="A68" s="11"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="26"/>
       <c r="D68" s="16"/>
       <c r="E68" s="16"/>
     </row>
     <row r="69" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A69" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B69" s="25">
-        <f>B68+1</f>
-        <v>67</v>
-      </c>
-      <c r="C69" s="26">
-        <v>0.95995833333333302</v>
-      </c>
+      <c r="A69" s="11"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="26"/>
       <c r="D69" s="16"/>
       <c r="E69" s="16"/>
     </row>
     <row r="70" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A70" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B70" s="25">
-        <f>B69+1</f>
-        <v>68</v>
-      </c>
-      <c r="C70" s="26">
-        <v>0.959666666666667</v>
-      </c>
+      <c r="A70" s="11"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="26"/>
       <c r="D70" s="16"/>
       <c r="E70" s="16"/>
     </row>
     <row r="71" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A71" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B71" s="25">
-        <f>B70+1</f>
-        <v>69</v>
-      </c>
-      <c r="C71" s="26">
-        <v>0.95937499999999998</v>
-      </c>
+      <c r="A71" s="11"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="26"/>
       <c r="D71" s="16"/>
       <c r="E71" s="16"/>
     </row>
     <row r="72" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A72" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B72" s="25">
-        <f>B71+1</f>
-        <v>70</v>
-      </c>
-      <c r="C72" s="26">
-        <v>0.95908333333333295</v>
-      </c>
+      <c r="A72" s="11"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="26"/>
       <c r="D72" s="16"/>
       <c r="E72" s="16"/>
     </row>
     <row r="73" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A73" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B73" s="25">
-        <f>B72+1</f>
-        <v>71</v>
-      </c>
-      <c r="C73" s="26">
-        <v>0.95879166666666704</v>
-      </c>
+      <c r="A73" s="11"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="26"/>
       <c r="D73" s="16"/>
       <c r="E73" s="16"/>
     </row>
     <row r="74" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A74" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B74" s="25">
-        <f>B73+1</f>
-        <v>72</v>
-      </c>
-      <c r="C74" s="26">
-        <v>0.95850000000000002</v>
-      </c>
+      <c r="A74" s="11"/>
+      <c r="B74" s="25"/>
+      <c r="C74" s="26"/>
       <c r="D74" s="16"/>
       <c r="E74" s="16"/>
     </row>
     <row r="75" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A75" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B75" s="25">
-        <f>B74+1</f>
-        <v>73</v>
-      </c>
-      <c r="C75" s="26">
-        <v>0.958208333333333</v>
-      </c>
+      <c r="A75" s="11"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="26"/>
       <c r="D75" s="16"/>
       <c r="E75" s="16"/>
     </row>
     <row r="76" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A76" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B76" s="25">
-        <f>B75+1</f>
-        <v>74</v>
-      </c>
-      <c r="C76" s="26">
-        <v>0.95791666666666697</v>
-      </c>
+      <c r="A76" s="11"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="26"/>
       <c r="D76" s="16"/>
       <c r="E76" s="16"/>
     </row>
     <row r="77" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A77" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B77" s="25">
-        <f>B76+1</f>
-        <v>75</v>
-      </c>
-      <c r="C77" s="26">
-        <v>0.95762499999999995</v>
-      </c>
+      <c r="A77" s="11"/>
+      <c r="B77" s="25"/>
+      <c r="C77" s="26"/>
       <c r="D77" s="16"/>
       <c r="E77" s="16"/>
     </row>
     <row r="78" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A78" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B78" s="25">
-        <f>B77+1</f>
-        <v>76</v>
-      </c>
-      <c r="C78" s="26">
-        <v>0.95733333333333304</v>
-      </c>
+      <c r="A78" s="11"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="26"/>
       <c r="D78" s="16"/>
       <c r="E78" s="16"/>
     </row>
     <row r="79" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A79" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B79" s="25">
-        <f>B78+1</f>
-        <v>77</v>
-      </c>
-      <c r="C79" s="26">
-        <v>0.95704166666666701</v>
-      </c>
+      <c r="A79" s="11"/>
+      <c r="B79" s="25"/>
+      <c r="C79" s="26"/>
       <c r="D79" s="16"/>
       <c r="E79" s="16"/>
     </row>
     <row r="80" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A80" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B80" s="25">
-        <f>B79+1</f>
-        <v>78</v>
-      </c>
-      <c r="C80" s="26">
-        <v>0.95674999999999999</v>
-      </c>
+      <c r="A80" s="11"/>
+      <c r="B80" s="25"/>
+      <c r="C80" s="26"/>
       <c r="D80" s="16"/>
       <c r="E80" s="16"/>
     </row>
     <row r="81" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A81" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B81" s="25">
-        <f>B80+1</f>
-        <v>79</v>
-      </c>
-      <c r="C81" s="26">
-        <v>0.95645833333333297</v>
-      </c>
+      <c r="A81" s="11"/>
+      <c r="B81" s="25"/>
+      <c r="C81" s="26"/>
       <c r="D81" s="16"/>
       <c r="E81" s="16"/>
     </row>
     <row r="82" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A82" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B82" s="25">
-        <f>B81+1</f>
-        <v>80</v>
-      </c>
-      <c r="C82" s="26">
-        <v>0.95616666666666705</v>
-      </c>
+      <c r="A82" s="11"/>
+      <c r="B82" s="25"/>
+      <c r="C82" s="26"/>
       <c r="D82" s="16"/>
       <c r="E82" s="16"/>
     </row>
     <row r="83" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A83" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B83" s="25">
-        <f>B82+1</f>
-        <v>81</v>
-      </c>
-      <c r="C83" s="26">
-        <v>0.95587500000000003</v>
-      </c>
+      <c r="A83" s="11"/>
+      <c r="B83" s="25"/>
+      <c r="C83" s="26"/>
       <c r="D83" s="16"/>
       <c r="E83" s="16"/>
     </row>
     <row r="84" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A84" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B84" s="25">
-        <f>B83+1</f>
-        <v>82</v>
-      </c>
-      <c r="C84" s="26">
-        <v>0.95558333333333301</v>
-      </c>
+      <c r="A84" s="11"/>
+      <c r="B84" s="25"/>
+      <c r="C84" s="26"/>
       <c r="D84" s="16"/>
       <c r="E84" s="16"/>
     </row>
     <row r="85" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A85" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B85" s="25">
-        <f>B84+1</f>
-        <v>83</v>
-      </c>
-      <c r="C85" s="26">
-        <v>0.95529166666666698</v>
-      </c>
+      <c r="A85" s="11"/>
+      <c r="B85" s="25"/>
+      <c r="C85" s="26"/>
       <c r="D85" s="16"/>
       <c r="E85" s="16"/>
     </row>
     <row r="86" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A86" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B86" s="25">
-        <f>B85+1</f>
-        <v>84</v>
-      </c>
-      <c r="C86" s="26">
-        <v>0.95499999999999996</v>
-      </c>
+      <c r="A86" s="11"/>
+      <c r="B86" s="25"/>
+      <c r="C86" s="26"/>
       <c r="D86" s="16"/>
       <c r="E86" s="16"/>
     </row>
     <row r="87" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A87" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B87" s="25">
-        <f>B86+1</f>
-        <v>85</v>
-      </c>
-      <c r="C87" s="26">
-        <v>0.95483333333333298</v>
-      </c>
+      <c r="A87" s="11"/>
+      <c r="B87" s="25"/>
+      <c r="C87" s="26"/>
       <c r="D87" s="16"/>
       <c r="E87" s="16"/>
     </row>
     <row r="88" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A88" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B88" s="25">
-        <f>B87+1</f>
-        <v>86</v>
-      </c>
-      <c r="C88" s="26">
-        <v>0.954666666666667</v>
-      </c>
+      <c r="A88" s="11"/>
+      <c r="B88" s="25"/>
+      <c r="C88" s="26"/>
       <c r="D88" s="16"/>
       <c r="E88" s="16"/>
     </row>
     <row r="89" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A89" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B89" s="25">
-        <f>B88+1</f>
-        <v>87</v>
-      </c>
-      <c r="C89" s="26">
-        <v>0.95450000000000002</v>
-      </c>
+      <c r="A89" s="11"/>
+      <c r="B89" s="25"/>
+      <c r="C89" s="26"/>
       <c r="D89" s="16"/>
       <c r="E89" s="16"/>
     </row>
     <row r="90" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A90" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B90" s="25">
-        <f>B89+1</f>
-        <v>88</v>
-      </c>
-      <c r="C90" s="26">
-        <v>0.95433333333333303</v>
-      </c>
+      <c r="A90" s="11"/>
+      <c r="B90" s="25"/>
+      <c r="C90" s="26"/>
       <c r="D90" s="16"/>
       <c r="E90" s="16"/>
     </row>
     <row r="91" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A91" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B91" s="25">
-        <f>B90+1</f>
-        <v>89</v>
-      </c>
-      <c r="C91" s="26">
-        <v>0.95416666666666705</v>
-      </c>
+      <c r="A91" s="11"/>
+      <c r="B91" s="25"/>
+      <c r="C91" s="26"/>
       <c r="D91" s="16"/>
       <c r="E91" s="16"/>
     </row>
     <row r="92" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A92" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B92" s="25">
-        <f>B91+1</f>
-        <v>90</v>
-      </c>
-      <c r="C92" s="26">
-        <v>0.95399999999999996</v>
-      </c>
+      <c r="A92" s="11"/>
+      <c r="B92" s="25"/>
+      <c r="C92" s="26"/>
       <c r="D92" s="16"/>
       <c r="E92" s="16"/>
     </row>
     <row r="93" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A93" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B93" s="25">
-        <f>B92+1</f>
-        <v>91</v>
-      </c>
-      <c r="C93" s="26">
-        <v>0.95383333333333298</v>
-      </c>
+      <c r="A93" s="11"/>
+      <c r="B93" s="25"/>
+      <c r="C93" s="26"/>
       <c r="D93" s="16"/>
       <c r="E93" s="16"/>
     </row>
     <row r="94" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A94" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B94" s="25">
-        <f>B93+1</f>
-        <v>92</v>
-      </c>
-      <c r="C94" s="26">
-        <v>0.953666666666667</v>
-      </c>
+      <c r="A94" s="11"/>
+      <c r="B94" s="25"/>
+      <c r="C94" s="26"/>
       <c r="D94" s="16"/>
       <c r="E94" s="16"/>
     </row>
     <row r="95" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A95" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B95" s="25">
-        <f>B94+1</f>
-        <v>93</v>
-      </c>
-      <c r="C95" s="26">
-        <v>0.95350000000000001</v>
-      </c>
+      <c r="A95" s="11"/>
+      <c r="B95" s="25"/>
+      <c r="C95" s="26"/>
       <c r="D95" s="16"/>
       <c r="E95" s="16"/>
     </row>
     <row r="96" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A96" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B96" s="25">
-        <f>B95+1</f>
-        <v>94</v>
-      </c>
-      <c r="C96" s="26">
-        <v>0.95333333333333303</v>
-      </c>
+      <c r="A96" s="11"/>
+      <c r="B96" s="25"/>
+      <c r="C96" s="26"/>
       <c r="D96" s="16"/>
       <c r="E96" s="16"/>
     </row>
     <row r="97" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A97" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B97" s="25">
-        <f>B96+1</f>
-        <v>95</v>
-      </c>
-      <c r="C97" s="26">
-        <v>0.95316666666666705</v>
-      </c>
+      <c r="A97" s="11"/>
+      <c r="B97" s="25"/>
+      <c r="C97" s="26"/>
       <c r="D97" s="16"/>
       <c r="E97" s="16"/>
     </row>
     <row r="98" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A98" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B98" s="25">
-        <f>B97+1</f>
-        <v>96</v>
-      </c>
-      <c r="C98" s="26">
-        <v>0.95299999999999996</v>
-      </c>
+      <c r="A98" s="11"/>
+      <c r="B98" s="25"/>
+      <c r="C98" s="26"/>
       <c r="D98" s="16"/>
       <c r="E98" s="16"/>
     </row>
     <row r="99" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A99" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B99" s="25">
-        <f>B98+1</f>
-        <v>97</v>
-      </c>
-      <c r="C99" s="26">
-        <v>0.95283333333333298</v>
-      </c>
+      <c r="A99" s="11"/>
+      <c r="B99" s="25"/>
+      <c r="C99" s="26"/>
       <c r="D99" s="16"/>
       <c r="E99" s="16"/>
     </row>
     <row r="100" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A100" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B100" s="25">
-        <f>B99+1</f>
-        <v>98</v>
-      </c>
-      <c r="C100" s="26">
-        <v>0.95266666666666699</v>
-      </c>
+      <c r="A100" s="11"/>
+      <c r="B100" s="25"/>
+      <c r="C100" s="26"/>
       <c r="D100" s="16"/>
       <c r="E100" s="16"/>
     </row>
     <row r="101" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A101" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B101" s="25">
-        <f>B100+1</f>
-        <v>99</v>
-      </c>
-      <c r="C101" s="26">
-        <v>0.95250000000000001</v>
-      </c>
+      <c r="A101" s="11"/>
+      <c r="B101" s="25"/>
+      <c r="C101" s="26"/>
       <c r="D101" s="16"/>
       <c r="E101" s="16"/>
     </row>
     <row r="102" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A102" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B102" s="25">
-        <f>B101+1</f>
-        <v>100</v>
-      </c>
-      <c r="C102" s="26">
-        <v>0.95233333333333303</v>
-      </c>
+      <c r="A102" s="11"/>
+      <c r="B102" s="25"/>
+      <c r="C102" s="26"/>
       <c r="D102" s="16"/>
       <c r="E102" s="16"/>
     </row>
     <row r="103" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A103" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B103" s="25">
-        <f>B102+1</f>
-        <v>101</v>
-      </c>
-      <c r="C103" s="26">
-        <v>0.95216666666666705</v>
-      </c>
+      <c r="A103" s="11"/>
+      <c r="B103" s="25"/>
+      <c r="C103" s="26"/>
       <c r="D103" s="16"/>
       <c r="E103" s="16"/>
     </row>
     <row r="104" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A104" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B104" s="25">
-        <f>B103+1</f>
-        <v>102</v>
-      </c>
-      <c r="C104" s="26">
-        <v>0.95199999999999996</v>
-      </c>
+      <c r="A104" s="11"/>
+      <c r="B104" s="25"/>
+      <c r="C104" s="26"/>
       <c r="D104" s="16"/>
       <c r="E104" s="16"/>
     </row>
     <row r="105" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A105" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B105" s="25">
-        <f>B104+1</f>
-        <v>103</v>
-      </c>
-      <c r="C105" s="26">
-        <v>0.95183333333333298</v>
-      </c>
+      <c r="A105" s="11"/>
+      <c r="B105" s="25"/>
+      <c r="C105" s="26"/>
       <c r="D105" s="16"/>
       <c r="E105" s="16"/>
     </row>
     <row r="106" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A106" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B106" s="25">
-        <f>B105+1</f>
-        <v>104</v>
-      </c>
-      <c r="C106" s="26">
-        <v>0.95166666666666699</v>
-      </c>
+      <c r="A106" s="11"/>
+      <c r="B106" s="25"/>
+      <c r="C106" s="26"/>
       <c r="D106" s="16"/>
       <c r="E106" s="16"/>
     </row>
     <row r="107" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A107" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B107" s="25">
-        <f>B106+1</f>
-        <v>105</v>
-      </c>
-      <c r="C107" s="26">
-        <v>0.95150000000000001</v>
-      </c>
+      <c r="A107" s="11"/>
+      <c r="B107" s="25"/>
+      <c r="C107" s="26"/>
       <c r="D107" s="16"/>
       <c r="E107" s="16"/>
     </row>
     <row r="108" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A108" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B108" s="25">
-        <f>B107+1</f>
-        <v>106</v>
-      </c>
-      <c r="C108" s="26">
-        <v>0.95133333333333303</v>
-      </c>
+      <c r="A108" s="11"/>
+      <c r="B108" s="25"/>
+      <c r="C108" s="26"/>
       <c r="D108" s="16"/>
       <c r="E108" s="16"/>
     </row>
     <row r="109" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A109" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B109" s="25">
-        <f>B108+1</f>
-        <v>107</v>
-      </c>
-      <c r="C109" s="26">
-        <v>0.95116666666666705</v>
-      </c>
+      <c r="A109" s="11"/>
+      <c r="B109" s="25"/>
+      <c r="C109" s="26"/>
       <c r="D109" s="16"/>
       <c r="E109" s="16"/>
     </row>
     <row r="110" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A110" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B110" s="25">
-        <f>B109+1</f>
-        <v>108</v>
-      </c>
-      <c r="C110" s="26">
-        <v>0.95099999999999996</v>
-      </c>
+      <c r="A110" s="11"/>
+      <c r="B110" s="25"/>
+      <c r="C110" s="26"/>
       <c r="D110" s="16"/>
       <c r="E110" s="16"/>
     </row>
     <row r="111" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A111" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B111" s="25">
-        <f>B110+1</f>
-        <v>109</v>
-      </c>
-      <c r="C111" s="26">
-        <v>0.95083333333333298</v>
-      </c>
+      <c r="A111" s="11"/>
+      <c r="B111" s="25"/>
+      <c r="C111" s="26"/>
       <c r="D111" s="16"/>
       <c r="E111" s="16"/>
     </row>
     <row r="112" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A112" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B112" s="25">
-        <f>B111+1</f>
-        <v>110</v>
-      </c>
-      <c r="C112" s="26">
-        <v>0.95066666666666699</v>
-      </c>
+      <c r="A112" s="11"/>
+      <c r="B112" s="25"/>
+      <c r="C112" s="26"/>
       <c r="D112" s="16"/>
       <c r="E112" s="16"/>
     </row>
     <row r="113" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A113" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B113" s="25">
-        <f>B112+1</f>
-        <v>111</v>
-      </c>
-      <c r="C113" s="26">
-        <v>0.95050000000000001</v>
-      </c>
+      <c r="A113" s="11"/>
+      <c r="B113" s="25"/>
+      <c r="C113" s="26"/>
       <c r="D113" s="16"/>
       <c r="E113" s="16"/>
     </row>
     <row r="114" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A114" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B114" s="25">
-        <f>B113+1</f>
-        <v>112</v>
-      </c>
-      <c r="C114" s="26">
-        <v>0.95033333333333303</v>
-      </c>
+      <c r="A114" s="11"/>
+      <c r="B114" s="25"/>
+      <c r="C114" s="26"/>
       <c r="D114" s="16"/>
       <c r="E114" s="16"/>
     </row>
     <row r="115" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A115" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B115" s="25">
-        <f>B114+1</f>
-        <v>113</v>
-      </c>
-      <c r="C115" s="26">
-        <v>0.95016666666666705</v>
-      </c>
+      <c r="A115" s="11"/>
+      <c r="B115" s="25"/>
+      <c r="C115" s="26"/>
       <c r="D115" s="16"/>
       <c r="E115" s="16"/>
     </row>
     <row r="116" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A116" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B116" s="25">
-        <f>B115+1</f>
-        <v>114</v>
-      </c>
-      <c r="C116" s="26">
-        <v>0.95</v>
-      </c>
+      <c r="A116" s="11"/>
+      <c r="B116" s="25"/>
+      <c r="C116" s="26"/>
       <c r="D116" s="16"/>
       <c r="E116" s="16"/>
     </row>
     <row r="117" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A117" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B117" s="25">
-        <f>B116+1</f>
-        <v>115</v>
-      </c>
-      <c r="C117" s="26">
-        <v>0.94983333333333297</v>
-      </c>
+      <c r="A117" s="11"/>
+      <c r="B117" s="25"/>
+      <c r="C117" s="26"/>
       <c r="D117" s="16"/>
       <c r="E117" s="16"/>
     </row>
     <row r="118" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A118" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B118" s="25">
-        <f>B117+1</f>
-        <v>116</v>
-      </c>
-      <c r="C118" s="26">
-        <v>0.94966666666666699</v>
-      </c>
+      <c r="A118" s="11"/>
+      <c r="B118" s="25"/>
+      <c r="C118" s="26"/>
       <c r="D118" s="16"/>
       <c r="E118" s="16"/>
     </row>
     <row r="119" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A119" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B119" s="25">
-        <f>B118+1</f>
-        <v>117</v>
-      </c>
-      <c r="C119" s="26">
-        <v>0.94950000000000001</v>
-      </c>
+      <c r="A119" s="11"/>
+      <c r="B119" s="25"/>
+      <c r="C119" s="26"/>
       <c r="D119" s="16"/>
       <c r="E119" s="16"/>
     </row>
     <row r="120" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A120" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B120" s="25">
-        <f>B119+1</f>
-        <v>118</v>
-      </c>
-      <c r="C120" s="26">
-        <v>0.94933333333333303</v>
-      </c>
+      <c r="A120" s="11"/>
+      <c r="B120" s="25"/>
+      <c r="C120" s="26"/>
       <c r="D120" s="16"/>
       <c r="E120" s="16"/>
     </row>
     <row r="121" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A121" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B121" s="25">
-        <f>B120+1</f>
-        <v>119</v>
-      </c>
-      <c r="C121" s="26">
-        <v>0.94916666666666705</v>
-      </c>
+      <c r="A121" s="11"/>
+      <c r="B121" s="25"/>
+      <c r="C121" s="26"/>
       <c r="D121" s="16"/>
       <c r="E121" s="16"/>
     </row>
     <row r="122" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A122" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B122" s="25">
-        <f>B121+1</f>
-        <v>120</v>
-      </c>
-      <c r="C122" s="26">
-        <v>0.94899999999999995</v>
-      </c>
+      <c r="A122" s="11"/>
+      <c r="B122" s="25"/>
+      <c r="C122" s="26"/>
       <c r="D122" s="16"/>
       <c r="E122" s="16"/>
     </row>
@@ -4834,8 +4234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView showGridLines="0" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4919,7 +4319,7 @@
         <v>50</v>
       </c>
       <c r="G2" s="23"/>
-      <c r="H2" s="58" t="s">
+      <c r="H2" s="57" t="s">
         <v>51</v>
       </c>
       <c r="I2" s="43">
@@ -4951,7 +4351,7 @@
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="59"/>
+      <c r="H3" s="58"/>
       <c r="I3" s="25">
         <v>50</v>
       </c>
@@ -4981,7 +4381,7 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="59"/>
+      <c r="H4" s="58"/>
       <c r="I4" s="25">
         <v>50</v>
       </c>
@@ -5011,7 +4411,7 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="59"/>
+      <c r="H5" s="58"/>
       <c r="I5" s="25">
         <v>50</v>
       </c>
@@ -5041,7 +4441,7 @@
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="59"/>
+      <c r="H6" s="58"/>
       <c r="I6" s="25">
         <v>50</v>
       </c>
@@ -5071,7 +4471,7 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="59"/>
+      <c r="H7" s="58"/>
       <c r="I7" s="25">
         <v>50</v>
       </c>
@@ -5101,7 +4501,7 @@
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="59"/>
+      <c r="H8" s="58"/>
       <c r="I8" s="25">
         <v>50</v>
       </c>
@@ -5131,7 +4531,7 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="59"/>
+      <c r="H9" s="58"/>
       <c r="I9" s="25">
         <v>50</v>
       </c>
@@ -5153,7 +4553,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="59"/>
+      <c r="H10" s="58"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -5181,7 +4581,7 @@
         <v>50</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="60" t="s">
+      <c r="H11" s="59" t="s">
         <v>70</v>
       </c>
       <c r="I11" s="25">
@@ -5215,7 +4615,7 @@
         <v>50</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="59"/>
+      <c r="H12" s="58"/>
       <c r="I12" s="25">
         <v>60</v>
       </c>
@@ -5247,7 +4647,7 @@
         <v>50</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="59"/>
+      <c r="H13" s="58"/>
       <c r="I13" s="25">
         <v>60</v>
       </c>
@@ -5269,7 +4669,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="59"/>
+      <c r="H14" s="58"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -5297,7 +4697,7 @@
         <v>50</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="61" t="s">
+      <c r="H15" s="60" t="s">
         <v>79</v>
       </c>
       <c r="I15" s="25">
@@ -5331,7 +4731,7 @@
         <v>50</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="59"/>
+      <c r="H16" s="58"/>
       <c r="I16" s="25">
         <v>70</v>
       </c>
@@ -5353,7 +4753,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="59"/>
+      <c r="H17" s="58"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -5381,7 +4781,7 @@
         <v>50</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="62" t="s">
+      <c r="H18" s="61" t="s">
         <v>87</v>
       </c>
       <c r="I18" s="25">
@@ -5415,7 +4815,7 @@
         <v>50</v>
       </c>
       <c r="G19" s="4"/>
-      <c r="H19" s="59"/>
+      <c r="H19" s="58"/>
       <c r="I19" s="25">
         <v>80</v>
       </c>
@@ -5447,7 +4847,7 @@
         <v>50</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="59"/>
+      <c r="H20" s="58"/>
       <c r="I20" s="25">
         <v>80</v>
       </c>
@@ -5479,7 +4879,7 @@
         <v>50</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="H21" s="59"/>
+      <c r="H21" s="58"/>
       <c r="I21" s="25">
         <v>80</v>
       </c>
@@ -5501,7 +4901,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="59"/>
+      <c r="H22" s="58"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -5529,7 +4929,7 @@
         <v>50</v>
       </c>
       <c r="G23" s="4"/>
-      <c r="H23" s="62" t="s">
+      <c r="H23" s="61" t="s">
         <v>94</v>
       </c>
       <c r="I23" s="25">
@@ -5563,7 +4963,7 @@
         <v>50</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="H24" s="59"/>
+      <c r="H24" s="58"/>
       <c r="I24" s="25">
         <v>90</v>
       </c>
@@ -5607,14 +5007,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" customHeight="1">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="45" t="s">

</xml_diff>

<commit_message>
KCP-50 - better descriptions of inputs, actually use the user's selection...
update kcp-models-master.xlsx to include all the :sub-text fields
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD876AEB-C1A9-4D38-B9B7-7B84A209839E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5273A929-D9C5-46C5-B04A-6A0CE1CDB5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="112">
   <si>
     <t>Notes</t>
   </si>
@@ -200,7 +200,7 @@
     <t>:v-radio</t>
   </si>
   <si>
-    <t>Stage 1a (or pT1a) – the cancer is small (4cm or smaller) and only inside the kidney</t>
+    <t>the cancer is small (4cm or smaller) and only inside the kidney</t>
   </si>
   <si>
     <t>[:p "The pathological stage of a kidney cancer tumour is a measure of its size and how far it has spread. This is determined by assessing cancer tissue removed during surgery."
@@ -222,7 +222,7 @@
     <t>pT1b</t>
   </si>
   <si>
-    <t>Stage 1b (or pT1b) – the cancer is small (between 4cm and 7 cm) and only inside the kidney</t>
+    <t>the cancer is small (between 4cm and 7 cm) and only inside the kidney</t>
   </si>
   <si>
     <t>:pT2a</t>
@@ -231,7 +231,7 @@
     <t>pT2a</t>
   </si>
   <si>
-    <t>Stage 2a (pT2a) - the cancer is between 7cm and 10cm and only inside the kidney</t>
+    <t>the cancer is between 7cm and 10cm and only inside the kidney</t>
   </si>
   <si>
     <t>:pT2b</t>
@@ -240,7 +240,7 @@
     <t>pT2b</t>
   </si>
   <si>
-    <t>Stage 2b (pT2b) – the cancer is larger than 10cm and only inside the kidney</t>
+    <t>the cancer is larger than 10cm and only inside the kidney</t>
   </si>
   <si>
     <t>:pT3a</t>
@@ -249,7 +249,7 @@
     <t>pT3a</t>
   </si>
   <si>
-    <t>Stage 3a (or pT3a) – the cancer is growing into the fat around the kidney, or into the renal vein</t>
+    <t>the cancer is growing into the fat around the kidney, or into the renal vein</t>
   </si>
   <si>
     <t>:pT3b</t>
@@ -258,7 +258,7 @@
     <t>pT3b</t>
   </si>
   <si>
-    <t>Stage 3b (or pT3b) - the cancer is growing into the vena cava in the tummy (abdomen)</t>
+    <t>the cancer is growing into the vena cava in the tummy (abdomen)</t>
   </si>
   <si>
     <t>:pT3c</t>
@@ -267,7 +267,7 @@
     <t>pT3c</t>
   </si>
   <si>
-    <t>Stage 3c (or pT3c) - the cancer is growing into the vena cava in the chest, or into the wall of the vena cava.</t>
+    <t>the cancer is growing into the vena cava in the chest, or into the wall of the vena cava.</t>
   </si>
   <si>
     <t>:pT4</t>
@@ -276,7 +276,7 @@
     <t>pT4</t>
   </si>
   <si>
-    <t>Stage 4 (or pT4) - the cancer has spread through the capsule that surrounds the kidney. It may have grown into the adrenal gland</t>
+    <t>the cancer has spread through the capsule that surrounds the kidney. It may have grown into the adrenal gland</t>
   </si>
   <si>
     <t>:n-stage</t>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>there were no lymph nodes found in the tumour samples removed at the time of surgery</t>
   </si>
   <si>
     <t>[:p "The regional lymph node status indicates if the cancer has spread to lymph nodes near the kidney. Lymph nodes are a network of glands found throughout the body that drain away waste fluid, waste products and damaged cells. They also fight infections."
@@ -305,10 +308,16 @@
     <t>pN0</t>
   </si>
   <si>
+    <t>no cancer was detected in any lymph nodes near the tumour</t>
+  </si>
+  <si>
     <t>:pN1</t>
   </si>
   <si>
     <t>pN1</t>
+  </si>
+  <si>
+    <t>cancer cells were detected in one or more lymph nodes near the tumour</t>
   </si>
   <si>
     <t>:tumor-size</t>
@@ -4258,8 +4267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4614,9 +4623,11 @@
       <c r="F11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="H11" s="59" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I11" s="25">
         <v>60</v>
@@ -4636,11 +4647,11 @@
         <v>74</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E12" s="25">
         <v>0</v>
@@ -4648,7 +4659,9 @@
       <c r="F12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="H12" s="58"/>
       <c r="I12" s="25">
         <v>60</v>
@@ -4656,7 +4669,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="44">
@@ -4668,11 +4681,11 @@
         <v>74</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E13" s="25">
         <v>0.92400000000000004</v>
@@ -4680,7 +4693,9 @@
       <c r="F13" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="H13" s="58"/>
       <c r="I13" s="25">
         <v>60</v>
@@ -4688,7 +4703,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="44">
@@ -4713,16 +4728,16 @@
     </row>
     <row r="15" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E15" s="25">
         <v>0</v>
@@ -4732,7 +4747,7 @@
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="60" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="I15" s="25">
         <v>70</v>
@@ -4740,7 +4755,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="9" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="44">
@@ -4749,14 +4764,14 @@
     </row>
     <row r="16" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="9" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E16" s="25">
         <v>0.39300000000000002</v>
@@ -4772,7 +4787,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="44">
@@ -4797,13 +4812,13 @@
     </row>
     <row r="18" spans="1:14" ht="119.25" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D18" s="25">
         <v>1</v>
@@ -4816,7 +4831,7 @@
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="61" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="I18" s="25">
         <v>80</v>
@@ -4833,10 +4848,10 @@
     </row>
     <row r="19" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="25">
@@ -4865,7 +4880,7 @@
     </row>
     <row r="20" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>34</v>
@@ -4897,10 +4912,10 @@
     </row>
     <row r="21" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="25">
@@ -4945,16 +4960,16 @@
     </row>
     <row r="23" spans="1:14" ht="45.4" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E23" s="25">
         <v>0</v>
@@ -4964,7 +4979,7 @@
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="61" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I23" s="25">
         <v>90</v>
@@ -4972,7 +4987,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="9" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="44">
@@ -4981,14 +4996,14 @@
     </row>
     <row r="24" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E24" s="25">
         <v>0.67800000000000005</v>
@@ -5004,7 +5019,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="9" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="44">
@@ -5042,7 +5057,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" customHeight="1">
       <c r="A1" s="62" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -5052,13 +5067,13 @@
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="45" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>

</xml_diff>

<commit_message>
KCP-80 - run the tests on CI, config tests "passing" (lots is commented out...)
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5273A929-D9C5-46C5-B04A-6A0CE1CDB5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7C0D0ED-829C-4FFB-A578-1F86854805BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="5" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="106">
   <si>
     <t>Notes</t>
   </si>
@@ -128,28 +128,22 @@
     <t>:optional</t>
   </si>
   <si>
-    <t>:age</t>
-  </si>
-  <si>
-    <t>:40+</t>
+    <t>:n-stage</t>
   </si>
   <si>
     <t>:no</t>
   </si>
   <si>
-    <t>:months-waiting</t>
-  </si>
-  <si>
-    <t>:mw-&lt;=6</t>
-  </si>
-  <si>
-    <t>:diabetes</t>
-  </si>
-  <si>
-    <t>:hla-mismatch</t>
-  </si>
-  <si>
-    <t>:3</t>
+    <t>:nuclear-grade</t>
+  </si>
+  <si>
+    <t>:t-stage</t>
+  </si>
+  <si>
+    <t>:tumor-size</t>
+  </si>
+  <si>
+    <t>:histologic-tumor-necrosis</t>
   </si>
   <si>
     <t>:factor-name</t>
@@ -183,9 +177,6 @@
   </si>
   <si>
     <t>:score</t>
-  </si>
-  <si>
-    <t>:t-stage</t>
   </si>
   <si>
     <t>:pT1a</t>
@@ -279,9 +270,6 @@
     <t>the cancer has spread through the capsule that surrounds the kidney. It may have grown into the adrenal gland</t>
   </si>
   <si>
-    <t>:n-stage</t>
-  </si>
-  <si>
     <t>:pNx</t>
   </si>
   <si>
@@ -318,9 +306,6 @@
   </si>
   <si>
     <t>cancer cells were detected in one or more lymph nodes near the tumour</t>
-  </si>
-  <si>
-    <t>:tumor-size</t>
   </si>
   <si>
     <t>:cm-&lt;10</t>
@@ -363,9 +348,6 @@
   </si>
   <si>
     <t>cm&gt;=10</t>
-  </si>
-  <si>
-    <t>:nuclear-grade</t>
   </si>
   <si>
     <t>:1</t>
@@ -439,10 +421,10 @@
     <t>:2</t>
   </si>
   <si>
+    <t>:3</t>
+  </si>
+  <si>
     <t>:4</t>
-  </si>
-  <si>
-    <t>:histologic-tumor-necrosis</t>
   </si>
   <si>
     <t>:No</t>
@@ -4144,7 +4126,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -4171,58 +4155,54 @@
       <c r="A2" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>31</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B3" s="35"/>
       <c r="C3" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>29</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B4" s="37"/>
       <c r="C4" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B5" s="37"/>
       <c r="C5" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" ht="17.100000000000001" customHeight="1">
-      <c r="A6" s="23"/>
+      <c r="A6" s="33" t="s">
+        <v>32</v>
+      </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="16"/>
+      <c r="C6" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16"/>
     </row>
@@ -4267,8 +4247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4296,66 +4276,66 @@
         <v>25</v>
       </c>
       <c r="C1" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="F1" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="G1" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="H1" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="I1" s="39" t="s">
         <v>39</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="39" t="s">
-        <v>41</v>
       </c>
       <c r="J1" s="39" t="s">
         <v>26</v>
       </c>
       <c r="K1" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="N1" s="41" t="s">
         <v>43</v>
-      </c>
-      <c r="M1" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" s="41" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="156.94999999999999" customHeight="1">
       <c r="A2" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="42" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>49</v>
       </c>
       <c r="E2" s="43">
         <v>0</v>
       </c>
       <c r="F2" s="42" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G2" s="58" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I2" s="43">
         <v>50</v>
@@ -4363,7 +4343,7 @@
       <c r="J2" s="23"/>
       <c r="K2" s="23"/>
       <c r="L2" s="42" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M2" s="23"/>
       <c r="N2" s="44">
@@ -4372,21 +4352,21 @@
     </row>
     <row r="3" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E3" s="25">
         <v>1.2430000000000001</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="58" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I3" s="25">
         <v>50</v>
@@ -4394,7 +4374,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="44">
@@ -4403,21 +4383,21 @@
     </row>
     <row r="4" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E4" s="25">
         <v>1.6479999999999999</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="58" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I4" s="25">
         <v>50</v>
@@ -4425,7 +4405,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="44">
@@ -4434,21 +4414,21 @@
     </row>
     <row r="5" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E5" s="25">
         <v>1.6479999999999999</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="58" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I5" s="25">
         <v>50</v>
@@ -4456,7 +4436,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="44">
@@ -4465,21 +4445,21 @@
     </row>
     <row r="6" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E6" s="25">
         <v>1.8959999999999999</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="58" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I6" s="25">
         <v>50</v>
@@ -4487,7 +4467,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="44">
@@ -4496,21 +4476,21 @@
     </row>
     <row r="7" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E7" s="25">
         <v>2.0139999999999998</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="58" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I7" s="25">
         <v>50</v>
@@ -4518,7 +4498,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="44">
@@ -4527,21 +4507,21 @@
     </row>
     <row r="8" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E8" s="25">
         <v>2.0139999999999998</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="58" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I8" s="25">
         <v>50</v>
@@ -4549,7 +4529,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="44">
@@ -4558,21 +4538,21 @@
     </row>
     <row r="9" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E9" s="25">
         <v>2.0139999999999998</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H9" s="58"/>
       <c r="I9" s="25">
@@ -4581,7 +4561,7 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="44">
@@ -4606,28 +4586,28 @@
     </row>
     <row r="11" spans="1:14" ht="126" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E11" s="25">
         <v>0</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H11" s="59" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I11" s="25">
         <v>60</v>
@@ -4635,7 +4615,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="44">
@@ -4644,23 +4624,23 @@
     </row>
     <row r="12" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E12" s="25">
         <v>0</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H12" s="58"/>
       <c r="I12" s="25">
@@ -4669,7 +4649,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="44">
@@ -4678,23 +4658,23 @@
     </row>
     <row r="13" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E13" s="25">
         <v>0.92400000000000004</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H13" s="58"/>
       <c r="I13" s="25">
@@ -4703,7 +4683,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="44">
@@ -4728,26 +4708,26 @@
     </row>
     <row r="15" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E15" s="25">
         <v>0</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="60" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I15" s="25">
         <v>70</v>
@@ -4755,7 +4735,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="44">
@@ -4764,20 +4744,20 @@
     </row>
     <row r="16" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E16" s="25">
         <v>0.39300000000000002</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="58"/>
@@ -4787,7 +4767,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="44">
@@ -4812,13 +4792,13 @@
     </row>
     <row r="18" spans="1:14" ht="119.25" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D18" s="25">
         <v>1</v>
@@ -4827,11 +4807,11 @@
         <v>0</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="61" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I18" s="25">
         <v>80</v>
@@ -4848,10 +4828,10 @@
     </row>
     <row r="19" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="25">
@@ -4861,7 +4841,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="58"/>
@@ -4880,10 +4860,10 @@
     </row>
     <row r="20" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="25">
@@ -4893,7 +4873,7 @@
         <v>0.64</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="58"/>
@@ -4912,10 +4892,10 @@
     </row>
     <row r="21" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>100</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="25">
@@ -4925,7 +4905,7 @@
         <v>1.3129999999999999</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="58"/>
@@ -4960,26 +4940,26 @@
     </row>
     <row r="23" spans="1:14" ht="45.4" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="E23" s="25">
         <v>0</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="61" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I23" s="25">
         <v>90</v>
@@ -4987,7 +4967,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="9" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="44">
@@ -4996,20 +4976,20 @@
     </row>
     <row r="24" spans="1:14" ht="17.100000000000001" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="9" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E24" s="25">
         <v>0.67800000000000005</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="58"/>
@@ -5019,7 +4999,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="9" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="44">
@@ -5057,7 +5037,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" customHeight="1">
       <c r="A1" s="62" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -5067,13 +5047,13 @@
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1">
       <c r="A2" s="45" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C2" s="45" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>

</xml_diff>

<commit_message>
KCP-76 - update model inputs page
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{180707A5-4DC6-4B3B-BE1A-926D279642D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD273C0C-1DD9-4201-85E1-027928685E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="5" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="4" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
     <t>assets/kidney/osm_logo.svg</t>
   </si>
   <si>
-    <t>Leibovich Score</t>
+    <t>Leibovich-Plus Score</t>
   </si>
   <si>
     <t>:label</t>
@@ -2115,7 +2115,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -4054,7 +4056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
KCP-90 - update printout based on feedback
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28409"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9D096E1-1831-45A5-8C56-572661716DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F150EB0C-282B-4FF8-9A48-0C23826D5C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
   </si>
   <si>
     <t>[:div "The pathological stage of a kidney cancer tumour is a measure of its size and how far it has spread. This is determined by assessing cancer tissue removed during surgery."
-   [:ul
+   [:ul { :class-name "more-info-list" }
       [:li "Stage 1a (or pT1a) – the cancer is small (4cm or smaller) and only inside the kidney"]
       [:li "Stage 1b (or pT1b) – the cancer is small (between 4cm and 7 cm) and only inside the kidney"]
       [:li "Stage 2a (pT2a) - the cancer is between 7cm and 10cm and only inside the kidney"]
@@ -288,8 +288,8 @@
     <t>there were no lymph nodes found in the tumour samples removed at the time of surgery</t>
   </si>
   <si>
-    <t>[:div "The regional lymph node status indicates if the cancer has spread to lymph nodes near the kidney. Lymph nodes are a network of glands found throughout the body that drain away waste products and fight infections. Lymph nodes near the kidney may be removed during surgery and tested for the presence of cancer."   
-    [:ul
+    <t>[:div "The regional lymph node status indicates if the cancer has spread to lymph nodes near the kidney. Lymph nodes are a network of glands found throughout the body that drain away waste products and fight infections. Lymph nodes near the kidney may be removed during surgery and tested for the presence of cancer.  However, it is common for no lymph nodes to be removed at the time of surgery and no further investigation to be required."
+    [:ul  { :class-name "more-info-list" }
         [:li "No investigation required (pNx) - There were no lymph nodes in the tissue removed at surgery. This is common if there are no noticeable lymph nodes present."]
         [:li "pN0 – No cancer was detected in any lymph nodes near the tumour."]
         [:li "pN1 – Cancer cells were detected in one or more lymph nodes near the tumour."]]
@@ -4188,8 +4188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E2" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
KCP-88 - update inputs based on feedback
</commit_message>
<xml_diff>
--- a/resources/kcp-models-master.xlsx
+++ b/resources/kcp-models-master.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28221"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD273C0C-1DD9-4201-85E1-027928685E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9D096E1-1831-45A5-8C56-572661716DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="4" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="126">
   <si>
     <t>Notes</t>
   </si>
@@ -200,7 +200,7 @@
     <t>the cancer is small (4cm or smaller) and only inside the kidney</t>
   </si>
   <si>
-    <t>[:p "The pathological stage of a kidney cancer tumour is a measure of its size and how far it has spread. This is determined by assessing cancer tissue removed during surgery."
+    <t>[:div "The pathological stage of a kidney cancer tumour is a measure of its size and how far it has spread. This is determined by assessing cancer tissue removed during surgery."
    [:ul
       [:li "Stage 1a (or pT1a) – the cancer is small (4cm or smaller) and only inside the kidney"]
       [:li "Stage 1b (or pT1b) – the cancer is small (between 4cm and 7 cm) and only inside the kidney"]
@@ -282,18 +282,21 @@
     <t>Regional lymph node status</t>
   </si>
   <si>
+    <t>Not requiring investigation</t>
+  </si>
+  <si>
+    <t>there were no lymph nodes found in the tumour samples removed at the time of surgery</t>
+  </si>
+  <si>
+    <t>[:div "The regional lymph node status indicates if the cancer has spread to lymph nodes near the kidney. Lymph nodes are a network of glands found throughout the body that drain away waste products and fight infections. Lymph nodes near the kidney may be removed during surgery and tested for the presence of cancer."   
+    [:ul
+        [:li "No investigation required (pNx) - There were no lymph nodes in the tissue removed at surgery. This is common if there are no noticeable lymph nodes present."]
+        [:li "pN0 – No cancer was detected in any lymph nodes near the tumour."]
+        [:li "pN1 – Cancer cells were detected in one or more lymph nodes near the tumour."]]
+]</t>
+  </si>
+  <si>
     <t>Unknown</t>
-  </si>
-  <si>
-    <t>there were no lymph nodes found in the tumour samples removed at the time of surgery</t>
-  </si>
-  <si>
-    <t>[:p "The regional lymph node status indicates if the cancer has spread to lymph nodes near the kidney. Lymph nodes are a network of glands found throughout the body that drain away waste fluid, waste products and damaged cells. They also fight infections."
-  [:ul
-      [:li "Unknown (pNx) – There were no lymph nodes found in the tumour samples removed at the time of surgery"]
-      [:li "pN0 – No cancer was detected in any lymph nodes near the tumour"]
-      [:li "pN1 – Cancer cells were detected in one or more lymph nodes near the tumour"]]
-]</t>
   </si>
   <si>
     <t>:pN0</t>
@@ -2115,7 +2118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -4185,8 +4188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4553,7 +4556,7 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="44">
@@ -4565,11 +4568,11 @@
         <v>27</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E12" s="53">
         <v>0</v>
@@ -4578,7 +4581,7 @@
         <v>49</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H12" s="46"/>
       <c r="I12" s="25">
@@ -4587,7 +4590,7 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="44">
@@ -4599,11 +4602,11 @@
         <v>27</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E13" s="53">
         <v>0.92400000000000004</v>
@@ -4612,7 +4615,7 @@
         <v>49</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H13" s="46"/>
       <c r="I13" s="25">
@@ -4621,7 +4624,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="44">
@@ -4649,13 +4652,13 @@
         <v>31</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E15" s="53">
         <v>0</v>
@@ -4665,7 +4668,7 @@
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="48" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I15" s="25">
         <v>70</v>
@@ -4673,7 +4676,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="44">
@@ -4685,11 +4688,11 @@
         <v>31</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E16" s="53">
         <v>0.39300000000000002</v>
@@ -4705,7 +4708,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="44">
@@ -4733,10 +4736,10 @@
         <v>29</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D18" s="25">
         <v>1</v>
@@ -4749,7 +4752,7 @@
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="49" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I18" s="25">
         <v>80</v>
@@ -4769,7 +4772,7 @@
         <v>29</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="25">
@@ -4801,7 +4804,7 @@
         <v>29</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="25">
@@ -4833,7 +4836,7 @@
         <v>29</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="25">
@@ -4881,13 +4884,13 @@
         <v>32</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E23" s="53">
         <v>0</v>
@@ -4897,7 +4900,7 @@
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="49" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I23" s="25">
         <v>90</v>
@@ -4905,7 +4908,7 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="44">
@@ -4917,11 +4920,11 @@
         <v>32</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E24" s="53">
         <v>0.67800000000000005</v>
@@ -4937,7 +4940,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="44">
@@ -4950,16 +4953,16 @@
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="53"/>
       <c r="F25" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="49" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I25" s="25">
         <v>100</v>
@@ -4977,13 +4980,13 @@
         <v>34</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E26" s="53">
         <v>0</v>
@@ -4999,7 +5002,7 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="44">
@@ -5011,11 +5014,11 @@
         <v>34</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E27" s="53">
         <v>0</v>
@@ -5031,7 +5034,7 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M27" s="4"/>
       <c r="N27" s="44">
@@ -5059,40 +5062,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
       <c r="A1" s="50" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D1" s="50" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F1" s="50" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G1" s="50" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H1" s="50" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I1" s="50" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J1" s="50" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K1" s="50" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L1" s="50" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -5100,7 +5103,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C2" s="51">
         <v>0</v>
@@ -5138,7 +5141,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C3" s="51">
         <v>0</v>
@@ -5176,7 +5179,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C4" s="51">
         <v>0</v>
@@ -5214,7 +5217,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C5" s="51">
         <v>0</v>
@@ -5252,7 +5255,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C6" s="51">
         <v>0</v>
@@ -5290,7 +5293,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C7" s="51">
         <v>0</v>
@@ -5328,7 +5331,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C8" s="51">
         <v>0</v>
@@ -5366,7 +5369,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C9" s="51">
         <v>0</v>
@@ -5404,7 +5407,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C10" s="51">
         <v>0</v>
@@ -5442,7 +5445,7 @@
         <v>34</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C11" s="51">
         <v>0</v>
@@ -5480,7 +5483,7 @@
         <v>35</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C12" s="51">
         <v>0</v>
@@ -5518,7 +5521,7 @@
         <v>36</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C13" s="51">
         <v>0</v>
@@ -5556,7 +5559,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C14" s="51">
         <v>0</v>
@@ -5594,7 +5597,7 @@
         <v>38</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C15" s="51">
         <v>0</v>
@@ -5632,7 +5635,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C16" s="51">
         <v>0</v>
@@ -5670,7 +5673,7 @@
         <v>40</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C17" s="51">
         <v>0</v>
@@ -5708,7 +5711,7 @@
         <v>41</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C18" s="51">
         <v>0</v>
@@ -5746,7 +5749,7 @@
         <v>42</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C19" s="51">
         <v>0</v>
@@ -5784,7 +5787,7 @@
         <v>43</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C20" s="51">
         <v>0</v>
@@ -5822,7 +5825,7 @@
         <v>44</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C21" s="51">
         <v>0</v>
@@ -5860,7 +5863,7 @@
         <v>45</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C22" s="51">
         <v>0</v>
@@ -5898,7 +5901,7 @@
         <v>46</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C23" s="51">
         <v>0</v>
@@ -5936,7 +5939,7 @@
         <v>47</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C24" s="51">
         <v>0</v>
@@ -5974,7 +5977,7 @@
         <v>48</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C25" s="51">
         <v>0</v>
@@ -6012,7 +6015,7 @@
         <v>49</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C26" s="51">
         <v>0</v>
@@ -6050,7 +6053,7 @@
         <v>50</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C27" s="51">
         <v>0</v>
@@ -6088,7 +6091,7 @@
         <v>51</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C28" s="51">
         <v>0</v>
@@ -6126,7 +6129,7 @@
         <v>52</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C29" s="51">
         <v>0</v>
@@ -6164,7 +6167,7 @@
         <v>53</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C30" s="51">
         <v>0</v>
@@ -6202,7 +6205,7 @@
         <v>54</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C31" s="51">
         <v>0</v>
@@ -6240,7 +6243,7 @@
         <v>55</v>
       </c>
       <c r="B32" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C32" s="51">
         <v>0</v>
@@ -6278,7 +6281,7 @@
         <v>56</v>
       </c>
       <c r="B33" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C33" s="51">
         <v>0.01</v>
@@ -6316,7 +6319,7 @@
         <v>57</v>
       </c>
       <c r="B34" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C34" s="51">
         <v>0.01</v>
@@ -6354,7 +6357,7 @@
         <v>58</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C35" s="51">
         <v>0.01</v>
@@ -6392,7 +6395,7 @@
         <v>59</v>
       </c>
       <c r="B36" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C36" s="51">
         <v>0.01</v>
@@ -6430,7 +6433,7 @@
         <v>60</v>
       </c>
       <c r="B37" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C37" s="51">
         <v>0.01</v>
@@ -6468,7 +6471,7 @@
         <v>61</v>
       </c>
       <c r="B38" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C38" s="51">
         <v>0.01</v>
@@ -6506,7 +6509,7 @@
         <v>62</v>
       </c>
       <c r="B39" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C39" s="51">
         <v>0.01</v>
@@ -6544,7 +6547,7 @@
         <v>63</v>
       </c>
       <c r="B40" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C40" s="51">
         <v>0.01</v>
@@ -6582,7 +6585,7 @@
         <v>64</v>
       </c>
       <c r="B41" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C41" s="51">
         <v>0.01</v>
@@ -6620,7 +6623,7 @@
         <v>65</v>
       </c>
       <c r="B42" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C42" s="51">
         <v>0.01</v>
@@ -6658,7 +6661,7 @@
         <v>66</v>
       </c>
       <c r="B43" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C43" s="51">
         <v>0.01</v>
@@ -6696,7 +6699,7 @@
         <v>67</v>
       </c>
       <c r="B44" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C44" s="51">
         <v>0.01</v>
@@ -6734,7 +6737,7 @@
         <v>68</v>
       </c>
       <c r="B45" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C45" s="51">
         <v>0.02</v>
@@ -6772,7 +6775,7 @@
         <v>69</v>
       </c>
       <c r="B46" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C46" s="51">
         <v>0.02</v>
@@ -6810,7 +6813,7 @@
         <v>70</v>
       </c>
       <c r="B47" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C47" s="51">
         <v>0.02</v>
@@ -6848,7 +6851,7 @@
         <v>71</v>
       </c>
       <c r="B48" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C48" s="51">
         <v>0.02</v>
@@ -6886,7 +6889,7 @@
         <v>72</v>
       </c>
       <c r="B49" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C49" s="51">
         <v>0.02</v>
@@ -6924,7 +6927,7 @@
         <v>73</v>
       </c>
       <c r="B50" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C50" s="51">
         <v>0.02</v>
@@ -6962,7 +6965,7 @@
         <v>74</v>
       </c>
       <c r="B51" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C51" s="51">
         <v>0.03</v>
@@ -7000,7 +7003,7 @@
         <v>75</v>
       </c>
       <c r="B52" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C52" s="51">
         <v>0.03</v>
@@ -7038,7 +7041,7 @@
         <v>76</v>
       </c>
       <c r="B53" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C53" s="51">
         <v>0.03</v>
@@ -7076,7 +7079,7 @@
         <v>77</v>
       </c>
       <c r="B54" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C54" s="51">
         <v>0.04</v>
@@ -7114,7 +7117,7 @@
         <v>78</v>
       </c>
       <c r="B55" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C55" s="51">
         <v>0.04</v>
@@ -7152,7 +7155,7 @@
         <v>79</v>
       </c>
       <c r="B56" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C56" s="51">
         <v>0.05</v>
@@ -7190,7 +7193,7 @@
         <v>80</v>
       </c>
       <c r="B57" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C57" s="51">
         <v>0.05</v>
@@ -7228,7 +7231,7 @@
         <v>81</v>
       </c>
       <c r="B58" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C58" s="51">
         <v>0.06</v>
@@ -7266,7 +7269,7 @@
         <v>82</v>
       </c>
       <c r="B59" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C59" s="51">
         <v>7.0000000000000007E-2</v>
@@ -7304,7 +7307,7 @@
         <v>83</v>
       </c>
       <c r="B60" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C60" s="51">
         <v>7.0000000000000007E-2</v>
@@ -7342,7 +7345,7 @@
         <v>84</v>
       </c>
       <c r="B61" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C61" s="51">
         <v>0.08</v>
@@ -7380,7 +7383,7 @@
         <v>85</v>
       </c>
       <c r="B62" s="51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C62" s="51">
         <v>0.09</v>
@@ -7418,7 +7421,7 @@
         <v>25</v>
       </c>
       <c r="B63" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C63" s="51">
         <v>0</v>
@@ -7456,7 +7459,7 @@
         <v>26</v>
       </c>
       <c r="B64" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C64" s="51">
         <v>0</v>
@@ -7494,7 +7497,7 @@
         <v>27</v>
       </c>
       <c r="B65" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C65" s="51">
         <v>0</v>
@@ -7532,7 +7535,7 @@
         <v>28</v>
       </c>
       <c r="B66" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C66" s="51">
         <v>0</v>
@@ -7570,7 +7573,7 @@
         <v>29</v>
       </c>
       <c r="B67" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C67" s="51">
         <v>0</v>
@@ -7608,7 +7611,7 @@
         <v>30</v>
       </c>
       <c r="B68" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C68" s="51">
         <v>0</v>
@@ -7646,7 +7649,7 @@
         <v>31</v>
       </c>
       <c r="B69" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C69" s="51">
         <v>0</v>
@@ -7684,7 +7687,7 @@
         <v>32</v>
       </c>
       <c r="B70" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C70" s="51">
         <v>0</v>
@@ -7722,7 +7725,7 @@
         <v>33</v>
       </c>
       <c r="B71" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C71" s="51">
         <v>0</v>
@@ -7760,7 +7763,7 @@
         <v>34</v>
       </c>
       <c r="B72" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C72" s="51">
         <v>0</v>
@@ -7798,7 +7801,7 @@
         <v>35</v>
       </c>
       <c r="B73" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C73" s="51">
         <v>0</v>
@@ -7836,7 +7839,7 @@
         <v>36</v>
       </c>
       <c r="B74" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C74" s="51">
         <v>0</v>
@@ -7874,7 +7877,7 @@
         <v>37</v>
       </c>
       <c r="B75" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C75" s="51">
         <v>0</v>
@@ -7912,7 +7915,7 @@
         <v>38</v>
       </c>
       <c r="B76" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C76" s="51">
         <v>0</v>
@@ -7950,7 +7953,7 @@
         <v>39</v>
       </c>
       <c r="B77" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C77" s="51">
         <v>0</v>
@@ -7988,7 +7991,7 @@
         <v>40</v>
       </c>
       <c r="B78" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C78" s="51">
         <v>0</v>
@@ -8026,7 +8029,7 @@
         <v>41</v>
       </c>
       <c r="B79" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C79" s="51">
         <v>0</v>
@@ -8064,7 +8067,7 @@
         <v>42</v>
       </c>
       <c r="B80" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C80" s="51">
         <v>0</v>
@@ -8102,7 +8105,7 @@
         <v>43</v>
       </c>
       <c r="B81" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C81" s="51">
         <v>0</v>
@@ -8140,7 +8143,7 @@
         <v>44</v>
       </c>
       <c r="B82" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C82" s="51">
         <v>0</v>
@@ -8178,7 +8181,7 @@
         <v>45</v>
       </c>
       <c r="B83" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C83" s="51">
         <v>0</v>
@@ -8216,7 +8219,7 @@
         <v>46</v>
       </c>
       <c r="B84" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C84" s="51">
         <v>0</v>
@@ -8254,7 +8257,7 @@
         <v>47</v>
       </c>
       <c r="B85" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C85" s="51">
         <v>0</v>
@@ -8292,7 +8295,7 @@
         <v>48</v>
       </c>
       <c r="B86" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C86" s="51">
         <v>0</v>
@@ -8330,7 +8333,7 @@
         <v>49</v>
       </c>
       <c r="B87" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C87" s="51">
         <v>0</v>
@@ -8368,7 +8371,7 @@
         <v>50</v>
       </c>
       <c r="B88" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C88" s="51">
         <v>0</v>
@@ -8406,7 +8409,7 @@
         <v>51</v>
       </c>
       <c r="B89" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C89" s="51">
         <v>0</v>
@@ -8444,7 +8447,7 @@
         <v>52</v>
       </c>
       <c r="B90" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C90" s="51">
         <v>0</v>
@@ -8482,7 +8485,7 @@
         <v>53</v>
       </c>
       <c r="B91" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C91" s="51">
         <v>0</v>
@@ -8520,7 +8523,7 @@
         <v>54</v>
       </c>
       <c r="B92" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C92" s="51">
         <v>0</v>
@@ -8558,7 +8561,7 @@
         <v>55</v>
       </c>
       <c r="B93" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C93" s="51">
         <v>0</v>
@@ -8596,7 +8599,7 @@
         <v>56</v>
       </c>
       <c r="B94" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C94" s="51">
         <v>0</v>
@@ -8634,7 +8637,7 @@
         <v>57</v>
       </c>
       <c r="B95" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C95" s="51">
         <v>0</v>
@@ -8672,7 +8675,7 @@
         <v>58</v>
       </c>
       <c r="B96" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C96" s="51">
         <v>0</v>
@@ -8710,7 +8713,7 @@
         <v>59</v>
       </c>
       <c r="B97" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C97" s="51">
         <v>0</v>
@@ -8748,7 +8751,7 @@
         <v>60</v>
       </c>
       <c r="B98" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C98" s="51">
         <v>0</v>
@@ -8786,7 +8789,7 @@
         <v>61</v>
       </c>
       <c r="B99" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C99" s="51">
         <v>0.01</v>
@@ -8824,7 +8827,7 @@
         <v>62</v>
       </c>
       <c r="B100" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C100" s="51">
         <v>0.01</v>
@@ -8862,7 +8865,7 @@
         <v>63</v>
       </c>
       <c r="B101" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C101" s="51">
         <v>0.01</v>
@@ -8900,7 +8903,7 @@
         <v>64</v>
       </c>
       <c r="B102" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C102" s="51">
         <v>0.01</v>
@@ -8938,7 +8941,7 @@
         <v>65</v>
       </c>
       <c r="B103" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C103" s="51">
         <v>0.01</v>
@@ -8976,7 +8979,7 @@
         <v>66</v>
       </c>
       <c r="B104" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C104" s="51">
         <v>0.01</v>
@@ -9014,7 +9017,7 @@
         <v>67</v>
       </c>
       <c r="B105" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C105" s="51">
         <v>0.01</v>
@@ -9052,7 +9055,7 @@
         <v>68</v>
       </c>
       <c r="B106" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C106" s="51">
         <v>0.01</v>
@@ -9090,7 +9093,7 @@
         <v>69</v>
       </c>
       <c r="B107" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C107" s="51">
         <v>0.01</v>
@@ -9128,7 +9131,7 @@
         <v>70</v>
       </c>
       <c r="B108" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C108" s="51">
         <v>0.01</v>
@@ -9166,7 +9169,7 @@
         <v>71</v>
       </c>
       <c r="B109" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C109" s="51">
         <v>0.01</v>
@@ -9204,7 +9207,7 @@
         <v>72</v>
       </c>
       <c r="B110" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C110" s="51">
         <v>0.01</v>
@@ -9242,7 +9245,7 @@
         <v>73</v>
       </c>
       <c r="B111" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C111" s="51">
         <v>0.02</v>
@@ -9280,7 +9283,7 @@
         <v>74</v>
       </c>
       <c r="B112" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C112" s="51">
         <v>0.02</v>
@@ -9318,7 +9321,7 @@
         <v>75</v>
       </c>
       <c r="B113" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C113" s="51">
         <v>0.02</v>
@@ -9356,7 +9359,7 @@
         <v>76</v>
       </c>
       <c r="B114" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C114" s="51">
         <v>0.02</v>
@@ -9394,7 +9397,7 @@
         <v>77</v>
       </c>
       <c r="B115" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C115" s="51">
         <v>0.03</v>
@@ -9432,7 +9435,7 @@
         <v>78</v>
       </c>
       <c r="B116" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C116" s="51">
         <v>0.03</v>
@@ -9470,7 +9473,7 @@
         <v>79</v>
       </c>
       <c r="B117" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C117" s="51">
         <v>0.03</v>
@@ -9508,7 +9511,7 @@
         <v>80</v>
       </c>
       <c r="B118" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C118" s="51">
         <v>0.04</v>
@@ -9546,7 +9549,7 @@
         <v>81</v>
       </c>
       <c r="B119" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C119" s="51">
         <v>0.04</v>
@@ -9584,7 +9587,7 @@
         <v>82</v>
       </c>
       <c r="B120" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C120" s="51">
         <v>0.05</v>
@@ -9622,7 +9625,7 @@
         <v>83</v>
       </c>
       <c r="B121" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C121" s="51">
         <v>0.05</v>
@@ -9660,7 +9663,7 @@
         <v>84</v>
       </c>
       <c r="B122" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C122" s="51">
         <v>0.06</v>
@@ -9698,7 +9701,7 @@
         <v>85</v>
       </c>
       <c r="B123" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C123" s="51">
         <v>7.0000000000000007E-2</v>

</xml_diff>